<commit_message>
mario draft : icons
</commit_message>
<xml_diff>
--- a/draft/Mario Kart 8 Deluxe Stat.xlsx
+++ b/draft/Mario Kart 8 Deluxe Stat.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\R\Github\source\content\blog\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\R\Github\source\draft\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="10785" activeTab="3"/>
+    <workbookView xWindow="3720" yWindow="0" windowWidth="27870" windowHeight="10785" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,14 @@
     <sheet name="Kart" sheetId="3" r:id="rId3"/>
     <sheet name="Glide" sheetId="5" r:id="rId4"/>
     <sheet name="Tire" sheetId="4" r:id="rId5"/>
+    <sheet name="Aliases" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2213" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="757">
   <si>
     <t>Characters</t>
   </si>
@@ -1927,6 +1928,390 @@
   </si>
   <si>
     <t>Speed_Land</t>
+  </si>
+  <si>
+    <t>Character</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Used Name</t>
+  </si>
+  <si>
+    <t>Alias 1</t>
+  </si>
+  <si>
+    <t>Alias 2</t>
+  </si>
+  <si>
+    <t>Alias 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baby Daisy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Peach </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Rosalina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lemmy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Mario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Baby Luigi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dry Bones </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Light Mii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toadette </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wendy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Isabelle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Koopa Troopa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lakitu </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bowser Jr.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Toad </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Shy Guy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Larry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat Peach </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inkling Girl </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Female Villager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peach </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Daisy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yoshi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanooki Mario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inkling Boy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Male Villager</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Ludwig </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Medium Mii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luigi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Iggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rosalina </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> King Boo </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal Mario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gold Mario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Pink Gold Peach</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waluigi </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Donkey Kong </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Roy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wario </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dry Bowser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bowser </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Morton </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Heavy Mii</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard Kart </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 300 SL Roadster </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> The Duke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pipe Frame </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Varmint </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> City Tripper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mach 8 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sports Coupe </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Inkstriker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Steel Driver </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Tri-Speeder </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bone Rattler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cat Cruiser </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comet </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Yoshi Bike </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teddy Buggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Circuit Special </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> B-Dasher </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> P-Wing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Badwagon </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GLA </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Standard ATV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prancer </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sport Bike </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Jet Bike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Biddybuggy </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Mr Scooty</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Landship </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Streetle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sneeker </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gold Standard </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Master Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W 25 Silver Arrow </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Standard Bike </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flame Rider </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wild Wiggler</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Blue Falcon </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Splat Buggy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tanooki Kart </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Koopa Clown</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Standard </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Blue Standard </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> GLA Tires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monster </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hot Monster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Roller </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Azure Roller</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slim </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Wood </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Crimson Slim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Slick </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cyber Slick</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metal </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gold Tires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Button </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Leaf Tires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Off-Road </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Retro Off-Road </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Triforce Tires</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sponge </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cushion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Super Glider </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Waddle Wing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Hylian Kite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud Glider </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parachute </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Flower Glider </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Paper Glider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wario Wing </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Plane Glider </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gold Glider</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peach Parasol </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Parafoil </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Bowser Kite </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> MKTV Parafoil</t>
+  </si>
+  <si>
+    <t>Kart</t>
+  </si>
+  <si>
+    <t>Glider</t>
   </si>
 </sst>
 </file>
@@ -2167,7 +2552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="118">
+  <cellXfs count="122">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -2277,45 +2662,49 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -2599,8 +2988,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1083"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="O3" sqref="O3:T48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2610,31 +2999,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="106" t="s">
+      <c r="A1" s="110" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="102" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="94"/>
-      <c r="D1" s="94"/>
-      <c r="E1" s="94"/>
-      <c r="F1" s="93" t="s">
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
+      <c r="F1" s="103" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="93" t="s">
+      <c r="G1" s="103" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="104" t="s">
+      <c r="H1" s="102" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="94"/>
-      <c r="J1" s="94"/>
-      <c r="K1" s="94"/>
-      <c r="L1" s="93" t="s">
+      <c r="I1" s="99"/>
+      <c r="J1" s="99"/>
+      <c r="K1" s="99"/>
+      <c r="L1" s="103" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="112" t="s">
+      <c r="M1" s="115" t="s">
         <v>6</v>
       </c>
       <c r="O1" s="4" t="str">
@@ -2645,7 +3034,7 @@
       <c r="V1" s="6"/>
     </row>
     <row r="2" spans="1:22" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="107"/>
+      <c r="A2" s="111"/>
       <c r="B2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2658,8 +3047,8 @@
       <c r="E2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="97"/>
-      <c r="G2" s="97"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
       <c r="H2" s="7" t="s">
         <v>7</v>
       </c>
@@ -2672,8 +3061,8 @@
       <c r="K2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="97"/>
-      <c r="M2" s="98"/>
+      <c r="L2" s="96"/>
+      <c r="M2" s="105"/>
       <c r="O2" s="9" t="s">
         <v>11</v>
       </c>
@@ -5075,161 +5464,161 @@
       <c r="A63" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B63" s="111" t="s">
+      <c r="B63" s="113" t="s">
         <v>138</v>
       </c>
-      <c r="C63" s="94"/>
-      <c r="D63" s="94"/>
-      <c r="E63" s="111" t="s">
+      <c r="C63" s="99"/>
+      <c r="D63" s="99"/>
+      <c r="E63" s="113" t="s">
         <v>139</v>
       </c>
-      <c r="F63" s="94"/>
-      <c r="G63" s="94"/>
-      <c r="H63" s="111" t="s">
+      <c r="F63" s="99"/>
+      <c r="G63" s="99"/>
+      <c r="H63" s="113" t="s">
         <v>140</v>
       </c>
-      <c r="I63" s="94"/>
-      <c r="J63" s="95"/>
+      <c r="I63" s="99"/>
+      <c r="J63" s="116"/>
     </row>
     <row r="64" spans="1:25" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="B64" s="109" t="s">
+      <c r="B64" s="107" t="s">
         <v>142</v>
       </c>
-      <c r="C64" s="97"/>
-      <c r="D64" s="97"/>
-      <c r="E64" s="109" t="s">
+      <c r="C64" s="96"/>
+      <c r="D64" s="96"/>
+      <c r="E64" s="107" t="s">
         <v>143</v>
       </c>
-      <c r="F64" s="97"/>
-      <c r="G64" s="97"/>
-      <c r="H64" s="109" t="s">
+      <c r="F64" s="96"/>
+      <c r="G64" s="96"/>
+      <c r="H64" s="107" t="s">
         <v>144</v>
       </c>
-      <c r="I64" s="97"/>
-      <c r="J64" s="98"/>
+      <c r="I64" s="96"/>
+      <c r="J64" s="105"/>
     </row>
     <row r="65" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="B65" s="108" t="s">
+      <c r="B65" s="106" t="s">
         <v>146</v>
       </c>
-      <c r="C65" s="97"/>
-      <c r="D65" s="97"/>
-      <c r="E65" s="108" t="s">
+      <c r="C65" s="96"/>
+      <c r="D65" s="96"/>
+      <c r="E65" s="106" t="s">
         <v>147</v>
       </c>
-      <c r="F65" s="97"/>
-      <c r="G65" s="97"/>
-      <c r="H65" s="108" t="s">
+      <c r="F65" s="96"/>
+      <c r="G65" s="96"/>
+      <c r="H65" s="106" t="s">
         <v>148</v>
       </c>
-      <c r="I65" s="97"/>
-      <c r="J65" s="98"/>
+      <c r="I65" s="96"/>
+      <c r="J65" s="105"/>
     </row>
     <row r="66" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B66" s="109" t="s">
+      <c r="B66" s="107" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="97"/>
-      <c r="D66" s="97"/>
-      <c r="E66" s="109" t="s">
+      <c r="C66" s="96"/>
+      <c r="D66" s="96"/>
+      <c r="E66" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="F66" s="97"/>
-      <c r="G66" s="97"/>
-      <c r="H66" s="109" t="s">
+      <c r="F66" s="96"/>
+      <c r="G66" s="96"/>
+      <c r="H66" s="107" t="s">
         <v>151</v>
       </c>
-      <c r="I66" s="97"/>
-      <c r="J66" s="98"/>
+      <c r="I66" s="96"/>
+      <c r="J66" s="105"/>
     </row>
     <row r="67" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="B67" s="108" t="s">
+      <c r="B67" s="106" t="s">
         <v>153</v>
       </c>
-      <c r="C67" s="97"/>
-      <c r="D67" s="97"/>
-      <c r="E67" s="108" t="s">
+      <c r="C67" s="96"/>
+      <c r="D67" s="96"/>
+      <c r="E67" s="106" t="s">
         <v>154</v>
       </c>
-      <c r="F67" s="97"/>
-      <c r="G67" s="97"/>
-      <c r="H67" s="108" t="s">
+      <c r="F67" s="96"/>
+      <c r="G67" s="96"/>
+      <c r="H67" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="I67" s="97"/>
-      <c r="J67" s="98"/>
+      <c r="I67" s="96"/>
+      <c r="J67" s="105"/>
     </row>
     <row r="68" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B68" s="109" t="s">
+      <c r="B68" s="107" t="s">
         <v>153</v>
       </c>
-      <c r="C68" s="97"/>
-      <c r="D68" s="97"/>
-      <c r="E68" s="109" t="s">
+      <c r="C68" s="96"/>
+      <c r="D68" s="96"/>
+      <c r="E68" s="107" t="s">
         <v>157</v>
       </c>
-      <c r="F68" s="97"/>
-      <c r="G68" s="97"/>
-      <c r="H68" s="109" t="s">
+      <c r="F68" s="96"/>
+      <c r="G68" s="96"/>
+      <c r="H68" s="107" t="s">
         <v>158</v>
       </c>
-      <c r="I68" s="97"/>
-      <c r="J68" s="98"/>
+      <c r="I68" s="96"/>
+      <c r="J68" s="105"/>
     </row>
     <row r="69" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B69" s="108" t="s">
+      <c r="B69" s="106" t="s">
         <v>159</v>
       </c>
-      <c r="C69" s="97"/>
-      <c r="D69" s="97"/>
-      <c r="E69" s="108" t="s">
+      <c r="C69" s="96"/>
+      <c r="D69" s="96"/>
+      <c r="E69" s="106" t="s">
         <v>160</v>
       </c>
-      <c r="F69" s="97"/>
-      <c r="G69" s="97"/>
-      <c r="H69" s="108" t="s">
+      <c r="F69" s="96"/>
+      <c r="G69" s="96"/>
+      <c r="H69" s="106" t="s">
         <v>161</v>
       </c>
-      <c r="I69" s="97"/>
-      <c r="J69" s="98"/>
+      <c r="I69" s="96"/>
+      <c r="J69" s="105"/>
     </row>
     <row r="70" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="B70" s="109" t="s">
+      <c r="B70" s="107" t="s">
         <v>159</v>
       </c>
-      <c r="C70" s="97"/>
-      <c r="D70" s="97"/>
-      <c r="E70" s="109" t="s">
+      <c r="C70" s="96"/>
+      <c r="D70" s="96"/>
+      <c r="E70" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="F70" s="97"/>
-      <c r="G70" s="97"/>
-      <c r="H70" s="109" t="s">
+      <c r="F70" s="96"/>
+      <c r="G70" s="96"/>
+      <c r="H70" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="I70" s="97"/>
-      <c r="J70" s="98"/>
+      <c r="I70" s="96"/>
+      <c r="J70" s="105"/>
       <c r="W70" s="5"/>
       <c r="X70" s="5"/>
       <c r="Y70" s="5"/>
@@ -5239,21 +5628,21 @@
       <c r="A71" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B71" s="108" t="s">
+      <c r="B71" s="106" t="s">
         <v>165</v>
       </c>
-      <c r="C71" s="97"/>
-      <c r="D71" s="97"/>
-      <c r="E71" s="108" t="s">
+      <c r="C71" s="96"/>
+      <c r="D71" s="96"/>
+      <c r="E71" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="F71" s="97"/>
-      <c r="G71" s="97"/>
-      <c r="H71" s="108" t="s">
+      <c r="F71" s="96"/>
+      <c r="G71" s="96"/>
+      <c r="H71" s="106" t="s">
         <v>167</v>
       </c>
-      <c r="I71" s="97"/>
-      <c r="J71" s="98"/>
+      <c r="I71" s="96"/>
+      <c r="J71" s="105"/>
       <c r="U71" s="5"/>
       <c r="V71" s="5"/>
       <c r="W71" s="5"/>
@@ -5265,21 +5654,21 @@
       <c r="A72" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="B72" s="109" t="s">
+      <c r="B72" s="107" t="s">
         <v>169</v>
       </c>
-      <c r="C72" s="97"/>
-      <c r="D72" s="97"/>
-      <c r="E72" s="109" t="s">
+      <c r="C72" s="96"/>
+      <c r="D72" s="96"/>
+      <c r="E72" s="107" t="s">
         <v>170</v>
       </c>
-      <c r="F72" s="97"/>
-      <c r="G72" s="97"/>
-      <c r="H72" s="109" t="s">
+      <c r="F72" s="96"/>
+      <c r="G72" s="96"/>
+      <c r="H72" s="107" t="s">
         <v>171</v>
       </c>
-      <c r="I72" s="97"/>
-      <c r="J72" s="98"/>
+      <c r="I72" s="96"/>
+      <c r="J72" s="105"/>
       <c r="U72" s="5"/>
       <c r="V72" s="5"/>
       <c r="W72" s="5"/>
@@ -5291,21 +5680,21 @@
       <c r="A73" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B73" s="108" t="s">
+      <c r="B73" s="106" t="s">
         <v>172</v>
       </c>
-      <c r="C73" s="97"/>
-      <c r="D73" s="97"/>
-      <c r="E73" s="108" t="s">
+      <c r="C73" s="96"/>
+      <c r="D73" s="96"/>
+      <c r="E73" s="106" t="s">
         <v>173</v>
       </c>
-      <c r="F73" s="97"/>
-      <c r="G73" s="97"/>
-      <c r="H73" s="108" t="s">
+      <c r="F73" s="96"/>
+      <c r="G73" s="96"/>
+      <c r="H73" s="106" t="s">
         <v>174</v>
       </c>
-      <c r="I73" s="97"/>
-      <c r="J73" s="98"/>
+      <c r="I73" s="96"/>
+      <c r="J73" s="105"/>
       <c r="U73" s="5"/>
       <c r="V73" s="5"/>
       <c r="W73" s="5"/>
@@ -5317,21 +5706,21 @@
       <c r="A74" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="B74" s="109" t="s">
+      <c r="B74" s="107" t="s">
         <v>176</v>
       </c>
-      <c r="C74" s="97"/>
-      <c r="D74" s="97"/>
-      <c r="E74" s="109" t="s">
+      <c r="C74" s="96"/>
+      <c r="D74" s="96"/>
+      <c r="E74" s="107" t="s">
         <v>177</v>
       </c>
-      <c r="F74" s="97"/>
-      <c r="G74" s="97"/>
-      <c r="H74" s="109" t="s">
+      <c r="F74" s="96"/>
+      <c r="G74" s="96"/>
+      <c r="H74" s="107" t="s">
         <v>178</v>
       </c>
-      <c r="I74" s="97"/>
-      <c r="J74" s="98"/>
+      <c r="I74" s="96"/>
+      <c r="J74" s="105"/>
       <c r="U74" s="5"/>
       <c r="V74" s="5"/>
       <c r="W74" s="5"/>
@@ -5343,21 +5732,21 @@
       <c r="A75" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B75" s="108" t="s">
+      <c r="B75" s="106" t="s">
         <v>179</v>
       </c>
-      <c r="C75" s="97"/>
-      <c r="D75" s="97"/>
-      <c r="E75" s="108" t="s">
+      <c r="C75" s="96"/>
+      <c r="D75" s="96"/>
+      <c r="E75" s="106" t="s">
         <v>180</v>
       </c>
-      <c r="F75" s="97"/>
-      <c r="G75" s="97"/>
-      <c r="H75" s="108" t="s">
+      <c r="F75" s="96"/>
+      <c r="G75" s="96"/>
+      <c r="H75" s="106" t="s">
         <v>181</v>
       </c>
-      <c r="I75" s="97"/>
-      <c r="J75" s="98"/>
+      <c r="I75" s="96"/>
+      <c r="J75" s="105"/>
       <c r="U75" s="5"/>
       <c r="V75" s="5"/>
       <c r="W75" s="5"/>
@@ -5369,21 +5758,21 @@
       <c r="A76" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="B76" s="109" t="s">
+      <c r="B76" s="107" t="s">
         <v>179</v>
       </c>
-      <c r="C76" s="97"/>
-      <c r="D76" s="97"/>
-      <c r="E76" s="109" t="s">
+      <c r="C76" s="96"/>
+      <c r="D76" s="96"/>
+      <c r="E76" s="107" t="s">
         <v>183</v>
       </c>
-      <c r="F76" s="97"/>
-      <c r="G76" s="97"/>
-      <c r="H76" s="109" t="s">
+      <c r="F76" s="96"/>
+      <c r="G76" s="96"/>
+      <c r="H76" s="107" t="s">
         <v>184</v>
       </c>
-      <c r="I76" s="97"/>
-      <c r="J76" s="98"/>
+      <c r="I76" s="96"/>
+      <c r="J76" s="105"/>
       <c r="U76" s="5"/>
       <c r="V76" s="5"/>
       <c r="W76" s="5"/>
@@ -5395,21 +5784,21 @@
       <c r="A77" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B77" s="108" t="s">
+      <c r="B77" s="106" t="s">
         <v>179</v>
       </c>
-      <c r="C77" s="97"/>
-      <c r="D77" s="97"/>
-      <c r="E77" s="108" t="s">
+      <c r="C77" s="96"/>
+      <c r="D77" s="96"/>
+      <c r="E77" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="F77" s="97"/>
-      <c r="G77" s="97"/>
-      <c r="H77" s="108" t="s">
+      <c r="F77" s="96"/>
+      <c r="G77" s="96"/>
+      <c r="H77" s="106" t="s">
         <v>186</v>
       </c>
-      <c r="I77" s="97"/>
-      <c r="J77" s="98"/>
+      <c r="I77" s="96"/>
+      <c r="J77" s="105"/>
       <c r="U77" s="5"/>
       <c r="V77" s="5"/>
       <c r="W77" s="5"/>
@@ -5421,21 +5810,21 @@
       <c r="A78" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="B78" s="109" t="s">
+      <c r="B78" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="C78" s="97"/>
-      <c r="D78" s="97"/>
-      <c r="E78" s="109" t="s">
+      <c r="C78" s="96"/>
+      <c r="D78" s="96"/>
+      <c r="E78" s="107" t="s">
         <v>189</v>
       </c>
-      <c r="F78" s="97"/>
-      <c r="G78" s="97"/>
-      <c r="H78" s="109" t="s">
+      <c r="F78" s="96"/>
+      <c r="G78" s="96"/>
+      <c r="H78" s="107" t="s">
         <v>190</v>
       </c>
-      <c r="I78" s="97"/>
-      <c r="J78" s="98"/>
+      <c r="I78" s="96"/>
+      <c r="J78" s="105"/>
       <c r="U78" s="5"/>
       <c r="V78" s="5"/>
       <c r="W78" s="5"/>
@@ -5447,21 +5836,21 @@
       <c r="A79" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B79" s="108" t="s">
+      <c r="B79" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="C79" s="97"/>
-      <c r="D79" s="97"/>
-      <c r="E79" s="108" t="s">
+      <c r="C79" s="96"/>
+      <c r="D79" s="96"/>
+      <c r="E79" s="106" t="s">
         <v>191</v>
       </c>
-      <c r="F79" s="97"/>
-      <c r="G79" s="97"/>
-      <c r="H79" s="108" t="s">
+      <c r="F79" s="96"/>
+      <c r="G79" s="96"/>
+      <c r="H79" s="106" t="s">
         <v>192</v>
       </c>
-      <c r="I79" s="97"/>
-      <c r="J79" s="98"/>
+      <c r="I79" s="96"/>
+      <c r="J79" s="105"/>
       <c r="U79" s="5"/>
       <c r="V79" s="5"/>
       <c r="W79" s="5"/>
@@ -5473,21 +5862,21 @@
       <c r="A80" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="B80" s="109" t="s">
+      <c r="B80" s="107" t="s">
         <v>194</v>
       </c>
-      <c r="C80" s="97"/>
-      <c r="D80" s="97"/>
-      <c r="E80" s="109" t="s">
+      <c r="C80" s="96"/>
+      <c r="D80" s="96"/>
+      <c r="E80" s="107" t="s">
         <v>195</v>
       </c>
-      <c r="F80" s="97"/>
-      <c r="G80" s="97"/>
-      <c r="H80" s="109" t="s">
+      <c r="F80" s="96"/>
+      <c r="G80" s="96"/>
+      <c r="H80" s="107" t="s">
         <v>196</v>
       </c>
-      <c r="I80" s="97"/>
-      <c r="J80" s="98"/>
+      <c r="I80" s="96"/>
+      <c r="J80" s="105"/>
       <c r="U80" s="5"/>
       <c r="V80" s="5"/>
       <c r="W80" s="5"/>
@@ -5499,21 +5888,21 @@
       <c r="A81" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B81" s="108" t="s">
+      <c r="B81" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="C81" s="97"/>
-      <c r="D81" s="97"/>
-      <c r="E81" s="108" t="s">
+      <c r="C81" s="96"/>
+      <c r="D81" s="96"/>
+      <c r="E81" s="106" t="s">
         <v>198</v>
       </c>
-      <c r="F81" s="97"/>
-      <c r="G81" s="97"/>
-      <c r="H81" s="108" t="s">
+      <c r="F81" s="96"/>
+      <c r="G81" s="96"/>
+      <c r="H81" s="106" t="s">
         <v>199</v>
       </c>
-      <c r="I81" s="97"/>
-      <c r="J81" s="98"/>
+      <c r="I81" s="96"/>
+      <c r="J81" s="105"/>
       <c r="U81" s="5"/>
       <c r="V81" s="5"/>
       <c r="W81" s="5"/>
@@ -5525,21 +5914,21 @@
       <c r="A82" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="B82" s="109" t="s">
+      <c r="B82" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="C82" s="97"/>
-      <c r="D82" s="97"/>
-      <c r="E82" s="109" t="s">
+      <c r="C82" s="96"/>
+      <c r="D82" s="96"/>
+      <c r="E82" s="107" t="s">
         <v>202</v>
       </c>
-      <c r="F82" s="97"/>
-      <c r="G82" s="97"/>
-      <c r="H82" s="109" t="s">
+      <c r="F82" s="96"/>
+      <c r="G82" s="96"/>
+      <c r="H82" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="I82" s="97"/>
-      <c r="J82" s="98"/>
+      <c r="I82" s="96"/>
+      <c r="J82" s="105"/>
       <c r="U82" s="5"/>
       <c r="V82" s="5"/>
       <c r="W82" s="5"/>
@@ -5551,21 +5940,21 @@
       <c r="A83" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="B83" s="110" t="s">
+      <c r="B83" s="114" t="s">
         <v>205</v>
       </c>
-      <c r="C83" s="103"/>
-      <c r="D83" s="103"/>
-      <c r="E83" s="110" t="s">
+      <c r="C83" s="101"/>
+      <c r="D83" s="101"/>
+      <c r="E83" s="114" t="s">
         <v>206</v>
       </c>
-      <c r="F83" s="103"/>
-      <c r="G83" s="103"/>
-      <c r="H83" s="110" t="s">
+      <c r="F83" s="101"/>
+      <c r="G83" s="101"/>
+      <c r="H83" s="114" t="s">
         <v>207</v>
       </c>
-      <c r="I83" s="103"/>
-      <c r="J83" s="105"/>
+      <c r="I83" s="101"/>
+      <c r="J83" s="117"/>
       <c r="U83" s="5"/>
       <c r="V83" s="5"/>
       <c r="W83" s="5"/>
@@ -5641,21 +6030,21 @@
       <c r="A90" s="43" t="s">
         <v>137</v>
       </c>
-      <c r="B90" s="111" t="s">
+      <c r="B90" s="113" t="s">
         <v>210</v>
       </c>
-      <c r="C90" s="94"/>
-      <c r="D90" s="94"/>
-      <c r="E90" s="111" t="s">
+      <c r="C90" s="99"/>
+      <c r="D90" s="99"/>
+      <c r="E90" s="113" t="s">
         <v>211</v>
       </c>
-      <c r="F90" s="94"/>
-      <c r="G90" s="94"/>
-      <c r="H90" s="111" t="s">
+      <c r="F90" s="99"/>
+      <c r="G90" s="99"/>
+      <c r="H90" s="113" t="s">
         <v>212</v>
       </c>
-      <c r="I90" s="94"/>
-      <c r="J90" s="95"/>
+      <c r="I90" s="99"/>
+      <c r="J90" s="116"/>
       <c r="K90" s="53"/>
       <c r="M90" s="6"/>
       <c r="U90" s="5"/>
@@ -5669,21 +6058,21 @@
       <c r="A91" s="44" t="s">
         <v>141</v>
       </c>
-      <c r="B91" s="109" t="s">
+      <c r="B91" s="107" t="s">
         <v>213</v>
       </c>
-      <c r="C91" s="97"/>
-      <c r="D91" s="97"/>
-      <c r="E91" s="109" t="s">
+      <c r="C91" s="96"/>
+      <c r="D91" s="96"/>
+      <c r="E91" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="F91" s="97"/>
-      <c r="G91" s="97"/>
-      <c r="H91" s="109" t="s">
+      <c r="F91" s="96"/>
+      <c r="G91" s="96"/>
+      <c r="H91" s="107" t="s">
         <v>215</v>
       </c>
-      <c r="I91" s="97"/>
-      <c r="J91" s="98"/>
+      <c r="I91" s="96"/>
+      <c r="J91" s="105"/>
       <c r="K91" s="53"/>
       <c r="M91" s="6"/>
       <c r="U91" s="5"/>
@@ -5697,21 +6086,21 @@
       <c r="A92" s="46" t="s">
         <v>145</v>
       </c>
-      <c r="B92" s="108" t="s">
+      <c r="B92" s="106" t="s">
         <v>216</v>
       </c>
-      <c r="C92" s="97"/>
-      <c r="D92" s="97"/>
-      <c r="E92" s="108" t="s">
+      <c r="C92" s="96"/>
+      <c r="D92" s="96"/>
+      <c r="E92" s="106" t="s">
         <v>214</v>
       </c>
-      <c r="F92" s="97"/>
-      <c r="G92" s="97"/>
-      <c r="H92" s="108" t="s">
+      <c r="F92" s="96"/>
+      <c r="G92" s="96"/>
+      <c r="H92" s="106" t="s">
         <v>215</v>
       </c>
-      <c r="I92" s="97"/>
-      <c r="J92" s="98"/>
+      <c r="I92" s="96"/>
+      <c r="J92" s="105"/>
       <c r="K92" s="53"/>
       <c r="M92" s="6"/>
       <c r="U92" s="5"/>
@@ -5725,21 +6114,21 @@
       <c r="A93" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="B93" s="109" t="s">
+      <c r="B93" s="107" t="s">
         <v>216</v>
       </c>
-      <c r="C93" s="97"/>
-      <c r="D93" s="97"/>
-      <c r="E93" s="109" t="s">
+      <c r="C93" s="96"/>
+      <c r="D93" s="96"/>
+      <c r="E93" s="107" t="s">
         <v>214</v>
       </c>
-      <c r="F93" s="97"/>
-      <c r="G93" s="97"/>
-      <c r="H93" s="109" t="s">
+      <c r="F93" s="96"/>
+      <c r="G93" s="96"/>
+      <c r="H93" s="107" t="s">
         <v>203</v>
       </c>
-      <c r="I93" s="97"/>
-      <c r="J93" s="98"/>
+      <c r="I93" s="96"/>
+      <c r="J93" s="105"/>
       <c r="K93" s="53"/>
       <c r="M93" s="6"/>
       <c r="U93" s="5"/>
@@ -5753,21 +6142,21 @@
       <c r="A94" s="46" t="s">
         <v>152</v>
       </c>
-      <c r="B94" s="108" t="s">
+      <c r="B94" s="106" t="s">
         <v>216</v>
       </c>
-      <c r="C94" s="97"/>
-      <c r="D94" s="97"/>
-      <c r="E94" s="108" t="s">
+      <c r="C94" s="96"/>
+      <c r="D94" s="96"/>
+      <c r="E94" s="106" t="s">
         <v>206</v>
       </c>
-      <c r="F94" s="97"/>
-      <c r="G94" s="97"/>
-      <c r="H94" s="108" t="s">
+      <c r="F94" s="96"/>
+      <c r="G94" s="96"/>
+      <c r="H94" s="106" t="s">
         <v>199</v>
       </c>
-      <c r="I94" s="97"/>
-      <c r="J94" s="98"/>
+      <c r="I94" s="96"/>
+      <c r="J94" s="105"/>
       <c r="K94" s="53"/>
       <c r="M94" s="6"/>
       <c r="U94" s="5"/>
@@ -5781,21 +6170,21 @@
       <c r="A95" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="107" t="s">
         <v>216</v>
       </c>
-      <c r="C95" s="97"/>
-      <c r="D95" s="97"/>
-      <c r="E95" s="109" t="s">
+      <c r="C95" s="96"/>
+      <c r="D95" s="96"/>
+      <c r="E95" s="107" t="s">
         <v>206</v>
       </c>
-      <c r="F95" s="97"/>
-      <c r="G95" s="97"/>
-      <c r="H95" s="109" t="s">
+      <c r="F95" s="96"/>
+      <c r="G95" s="96"/>
+      <c r="H95" s="107" t="s">
         <v>199</v>
       </c>
-      <c r="I95" s="97"/>
-      <c r="J95" s="98"/>
+      <c r="I95" s="96"/>
+      <c r="J95" s="105"/>
       <c r="K95" s="53"/>
       <c r="M95" s="6"/>
       <c r="U95" s="5"/>
@@ -5809,21 +6198,21 @@
       <c r="A96" s="46" t="s">
         <v>13</v>
       </c>
-      <c r="B96" s="108" t="s">
+      <c r="B96" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="C96" s="97"/>
-      <c r="D96" s="97"/>
-      <c r="E96" s="108" t="s">
+      <c r="C96" s="96"/>
+      <c r="D96" s="96"/>
+      <c r="E96" s="106" t="s">
         <v>218</v>
       </c>
-      <c r="F96" s="97"/>
-      <c r="G96" s="97"/>
-      <c r="H96" s="108" t="s">
+      <c r="F96" s="96"/>
+      <c r="G96" s="96"/>
+      <c r="H96" s="106" t="s">
         <v>219</v>
       </c>
-      <c r="I96" s="97"/>
-      <c r="J96" s="98"/>
+      <c r="I96" s="96"/>
+      <c r="J96" s="105"/>
       <c r="K96" s="53"/>
       <c r="M96" s="6"/>
       <c r="U96" s="5"/>
@@ -5837,21 +6226,21 @@
       <c r="A97" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="B97" s="109" t="s">
+      <c r="B97" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="C97" s="97"/>
-      <c r="D97" s="97"/>
-      <c r="E97" s="109" t="s">
+      <c r="C97" s="96"/>
+      <c r="D97" s="96"/>
+      <c r="E97" s="107" t="s">
         <v>218</v>
       </c>
-      <c r="F97" s="97"/>
-      <c r="G97" s="97"/>
-      <c r="H97" s="109" t="s">
+      <c r="F97" s="96"/>
+      <c r="G97" s="96"/>
+      <c r="H97" s="107" t="s">
         <v>219</v>
       </c>
-      <c r="I97" s="97"/>
-      <c r="J97" s="98"/>
+      <c r="I97" s="96"/>
+      <c r="J97" s="105"/>
       <c r="K97" s="53"/>
       <c r="M97" s="6"/>
       <c r="U97" s="5"/>
@@ -5865,21 +6254,21 @@
       <c r="A98" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="B98" s="108" t="s">
+      <c r="B98" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="C98" s="97"/>
-      <c r="D98" s="97"/>
-      <c r="E98" s="108" t="s">
+      <c r="C98" s="96"/>
+      <c r="D98" s="96"/>
+      <c r="E98" s="106" t="s">
         <v>218</v>
       </c>
-      <c r="F98" s="97"/>
-      <c r="G98" s="97"/>
-      <c r="H98" s="108" t="s">
+      <c r="F98" s="96"/>
+      <c r="G98" s="96"/>
+      <c r="H98" s="106" t="s">
         <v>220</v>
       </c>
-      <c r="I98" s="97"/>
-      <c r="J98" s="98"/>
+      <c r="I98" s="96"/>
+      <c r="J98" s="105"/>
       <c r="K98" s="53"/>
       <c r="M98" s="6"/>
       <c r="U98" s="5"/>
@@ -5893,21 +6282,21 @@
       <c r="A99" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="B99" s="109" t="s">
+      <c r="B99" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="C99" s="97"/>
-      <c r="D99" s="97"/>
-      <c r="E99" s="109" t="s">
+      <c r="C99" s="96"/>
+      <c r="D99" s="96"/>
+      <c r="E99" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="F99" s="97"/>
-      <c r="G99" s="97"/>
-      <c r="H99" s="109" t="s">
+      <c r="F99" s="96"/>
+      <c r="G99" s="96"/>
+      <c r="H99" s="107" t="s">
         <v>186</v>
       </c>
-      <c r="I99" s="97"/>
-      <c r="J99" s="98"/>
+      <c r="I99" s="96"/>
+      <c r="J99" s="105"/>
       <c r="K99" s="53"/>
       <c r="M99" s="6"/>
       <c r="U99" s="5"/>
@@ -5921,21 +6310,21 @@
       <c r="A100" s="46" t="s">
         <v>30</v>
       </c>
-      <c r="B100" s="108" t="s">
+      <c r="B100" s="106" t="s">
         <v>217</v>
       </c>
-      <c r="C100" s="97"/>
-      <c r="D100" s="97"/>
-      <c r="E100" s="108" t="s">
+      <c r="C100" s="96"/>
+      <c r="D100" s="96"/>
+      <c r="E100" s="106" t="s">
         <v>221</v>
       </c>
-      <c r="F100" s="97"/>
-      <c r="G100" s="97"/>
-      <c r="H100" s="108" t="s">
+      <c r="F100" s="96"/>
+      <c r="G100" s="96"/>
+      <c r="H100" s="106" t="s">
         <v>186</v>
       </c>
-      <c r="I100" s="97"/>
-      <c r="J100" s="98"/>
+      <c r="I100" s="96"/>
+      <c r="J100" s="105"/>
       <c r="K100" s="53"/>
       <c r="M100" s="6"/>
       <c r="U100" s="5"/>
@@ -5949,21 +6338,21 @@
       <c r="A101" s="44" t="s">
         <v>175</v>
       </c>
-      <c r="B101" s="109" t="s">
+      <c r="B101" s="107" t="s">
         <v>217</v>
       </c>
-      <c r="C101" s="97"/>
-      <c r="D101" s="97"/>
-      <c r="E101" s="109" t="s">
+      <c r="C101" s="96"/>
+      <c r="D101" s="96"/>
+      <c r="E101" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="F101" s="97"/>
-      <c r="G101" s="97"/>
-      <c r="H101" s="109" t="s">
+      <c r="F101" s="96"/>
+      <c r="G101" s="96"/>
+      <c r="H101" s="107" t="s">
         <v>223</v>
       </c>
-      <c r="I101" s="97"/>
-      <c r="J101" s="98"/>
+      <c r="I101" s="96"/>
+      <c r="J101" s="105"/>
       <c r="K101" s="53"/>
       <c r="M101" s="6"/>
       <c r="U101" s="5"/>
@@ -5977,21 +6366,21 @@
       <c r="A102" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="B102" s="108" t="s">
+      <c r="B102" s="106" t="s">
         <v>201</v>
       </c>
-      <c r="C102" s="97"/>
-      <c r="D102" s="97"/>
-      <c r="E102" s="108" t="s">
+      <c r="C102" s="96"/>
+      <c r="D102" s="96"/>
+      <c r="E102" s="106" t="s">
         <v>222</v>
       </c>
-      <c r="F102" s="97"/>
-      <c r="G102" s="97"/>
-      <c r="H102" s="108" t="s">
+      <c r="F102" s="96"/>
+      <c r="G102" s="96"/>
+      <c r="H102" s="106" t="s">
         <v>223</v>
       </c>
-      <c r="I102" s="97"/>
-      <c r="J102" s="98"/>
+      <c r="I102" s="96"/>
+      <c r="J102" s="105"/>
       <c r="K102" s="53"/>
       <c r="M102" s="6"/>
       <c r="U102" s="5"/>
@@ -6005,21 +6394,21 @@
       <c r="A103" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="B103" s="109" t="s">
+      <c r="B103" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="C103" s="97"/>
-      <c r="D103" s="97"/>
-      <c r="E103" s="109" t="s">
+      <c r="C103" s="96"/>
+      <c r="D103" s="96"/>
+      <c r="E103" s="107" t="s">
         <v>222</v>
       </c>
-      <c r="F103" s="97"/>
-      <c r="G103" s="97"/>
-      <c r="H103" s="109" t="s">
+      <c r="F103" s="96"/>
+      <c r="G103" s="96"/>
+      <c r="H103" s="107" t="s">
         <v>224</v>
       </c>
-      <c r="I103" s="97"/>
-      <c r="J103" s="98"/>
+      <c r="I103" s="96"/>
+      <c r="J103" s="105"/>
       <c r="K103" s="53"/>
       <c r="L103" s="52"/>
       <c r="M103" s="6"/>
@@ -6034,21 +6423,21 @@
       <c r="A104" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="B104" s="108" t="s">
+      <c r="B104" s="106" t="s">
         <v>201</v>
       </c>
-      <c r="C104" s="97"/>
-      <c r="D104" s="97"/>
-      <c r="E104" s="108" t="s">
+      <c r="C104" s="96"/>
+      <c r="D104" s="96"/>
+      <c r="E104" s="106" t="s">
         <v>225</v>
       </c>
-      <c r="F104" s="97"/>
-      <c r="G104" s="97"/>
-      <c r="H104" s="108" t="s">
+      <c r="F104" s="96"/>
+      <c r="G104" s="96"/>
+      <c r="H104" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="I104" s="97"/>
-      <c r="J104" s="98"/>
+      <c r="I104" s="96"/>
+      <c r="J104" s="105"/>
       <c r="K104" s="53"/>
       <c r="L104" s="52"/>
       <c r="M104" s="6"/>
@@ -6063,21 +6452,21 @@
       <c r="A105" s="44" t="s">
         <v>187</v>
       </c>
-      <c r="B105" s="109" t="s">
+      <c r="B105" s="107" t="s">
         <v>201</v>
       </c>
-      <c r="C105" s="97"/>
-      <c r="D105" s="97"/>
-      <c r="E105" s="109" t="s">
+      <c r="C105" s="96"/>
+      <c r="D105" s="96"/>
+      <c r="E105" s="107" t="s">
         <v>225</v>
       </c>
-      <c r="F105" s="97"/>
-      <c r="G105" s="97"/>
-      <c r="H105" s="109" t="s">
+      <c r="F105" s="96"/>
+      <c r="G105" s="96"/>
+      <c r="H105" s="107" t="s">
         <v>164</v>
       </c>
-      <c r="I105" s="97"/>
-      <c r="J105" s="98"/>
+      <c r="I105" s="96"/>
+      <c r="J105" s="105"/>
       <c r="K105" s="53"/>
       <c r="L105" s="52"/>
       <c r="M105" s="6"/>
@@ -6092,21 +6481,21 @@
       <c r="A106" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B106" s="108" t="s">
+      <c r="B106" s="106" t="s">
         <v>201</v>
       </c>
-      <c r="C106" s="97"/>
-      <c r="D106" s="97"/>
-      <c r="E106" s="108" t="s">
+      <c r="C106" s="96"/>
+      <c r="D106" s="96"/>
+      <c r="E106" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="F106" s="97"/>
-      <c r="G106" s="97"/>
-      <c r="H106" s="108" t="s">
+      <c r="F106" s="96"/>
+      <c r="G106" s="96"/>
+      <c r="H106" s="106" t="s">
         <v>155</v>
       </c>
-      <c r="I106" s="97"/>
-      <c r="J106" s="98"/>
+      <c r="I106" s="96"/>
+      <c r="J106" s="105"/>
       <c r="K106" s="53"/>
       <c r="L106" s="52"/>
       <c r="M106" s="6"/>
@@ -6121,21 +6510,21 @@
       <c r="A107" s="44" t="s">
         <v>193</v>
       </c>
-      <c r="B107" s="109" t="s">
+      <c r="B107" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="C107" s="97"/>
-      <c r="D107" s="97"/>
-      <c r="E107" s="109" t="s">
+      <c r="C107" s="96"/>
+      <c r="D107" s="96"/>
+      <c r="E107" s="107" t="s">
         <v>166</v>
       </c>
-      <c r="F107" s="97"/>
-      <c r="G107" s="97"/>
-      <c r="H107" s="109" t="s">
+      <c r="F107" s="96"/>
+      <c r="G107" s="96"/>
+      <c r="H107" s="107" t="s">
         <v>155</v>
       </c>
-      <c r="I107" s="97"/>
-      <c r="J107" s="98"/>
+      <c r="I107" s="96"/>
+      <c r="J107" s="105"/>
       <c r="K107" s="53"/>
       <c r="L107" s="52"/>
       <c r="M107" s="6"/>
@@ -6150,21 +6539,21 @@
       <c r="A108" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="B108" s="108" t="s">
+      <c r="B108" s="106" t="s">
         <v>188</v>
       </c>
-      <c r="C108" s="97"/>
-      <c r="D108" s="97"/>
-      <c r="E108" s="108" t="s">
+      <c r="C108" s="96"/>
+      <c r="D108" s="96"/>
+      <c r="E108" s="106" t="s">
         <v>166</v>
       </c>
-      <c r="F108" s="97"/>
-      <c r="G108" s="97"/>
-      <c r="H108" s="108" t="s">
+      <c r="F108" s="96"/>
+      <c r="G108" s="96"/>
+      <c r="H108" s="106" t="s">
         <v>226</v>
       </c>
-      <c r="I108" s="97"/>
-      <c r="J108" s="98"/>
+      <c r="I108" s="96"/>
+      <c r="J108" s="105"/>
       <c r="K108" s="53"/>
       <c r="L108" s="52"/>
       <c r="M108" s="6"/>
@@ -6179,21 +6568,21 @@
       <c r="A109" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="B109" s="109" t="s">
+      <c r="B109" s="107" t="s">
         <v>188</v>
       </c>
-      <c r="C109" s="97"/>
-      <c r="D109" s="97"/>
-      <c r="E109" s="109" t="s">
+      <c r="C109" s="96"/>
+      <c r="D109" s="96"/>
+      <c r="E109" s="107" t="s">
         <v>150</v>
       </c>
-      <c r="F109" s="97"/>
-      <c r="G109" s="97"/>
-      <c r="H109" s="109" t="s">
+      <c r="F109" s="96"/>
+      <c r="G109" s="96"/>
+      <c r="H109" s="107" t="s">
         <v>227</v>
       </c>
-      <c r="I109" s="97"/>
-      <c r="J109" s="98"/>
+      <c r="I109" s="96"/>
+      <c r="J109" s="105"/>
       <c r="K109" s="53"/>
       <c r="L109" s="52"/>
       <c r="M109" s="6"/>
@@ -6208,21 +6597,21 @@
       <c r="A110" s="48" t="s">
         <v>204</v>
       </c>
-      <c r="B110" s="110" t="s">
+      <c r="B110" s="114" t="s">
         <v>188</v>
       </c>
-      <c r="C110" s="103"/>
-      <c r="D110" s="103"/>
-      <c r="E110" s="110" t="s">
+      <c r="C110" s="101"/>
+      <c r="D110" s="101"/>
+      <c r="E110" s="114" t="s">
         <v>150</v>
       </c>
-      <c r="F110" s="103"/>
-      <c r="G110" s="103"/>
-      <c r="H110" s="110" t="s">
+      <c r="F110" s="101"/>
+      <c r="G110" s="101"/>
+      <c r="H110" s="114" t="s">
         <v>227</v>
       </c>
-      <c r="I110" s="103"/>
-      <c r="J110" s="105"/>
+      <c r="I110" s="101"/>
+      <c r="J110" s="117"/>
       <c r="K110" s="53"/>
       <c r="L110" s="52"/>
       <c r="M110" s="52"/>
@@ -7832,16 +8221,16 @@
       <c r="W197" s="5"/>
     </row>
     <row r="198" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A198" s="106" t="s">
+      <c r="A198" s="110" t="s">
         <v>1</v>
       </c>
-      <c r="B198" s="104" t="s">
+      <c r="B198" s="102" t="s">
         <v>285</v>
       </c>
-      <c r="C198" s="94"/>
-      <c r="D198" s="94"/>
-      <c r="E198" s="94"/>
-      <c r="F198" s="113" t="s">
+      <c r="C198" s="99"/>
+      <c r="D198" s="99"/>
+      <c r="E198" s="99"/>
+      <c r="F198" s="112" t="s">
         <v>10</v>
       </c>
       <c r="J198" s="60"/>
@@ -7851,16 +8240,16 @@
       <c r="W198" s="5"/>
     </row>
     <row r="199" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A199" s="107"/>
-      <c r="B199" s="114" t="s">
+      <c r="A199" s="111"/>
+      <c r="B199" s="108" t="s">
         <v>286</v>
       </c>
-      <c r="C199" s="97"/>
-      <c r="D199" s="114" t="s">
+      <c r="C199" s="96"/>
+      <c r="D199" s="108" t="s">
         <v>287</v>
       </c>
-      <c r="E199" s="97"/>
-      <c r="F199" s="98"/>
+      <c r="E199" s="96"/>
+      <c r="F199" s="105"/>
       <c r="U199" s="5"/>
       <c r="V199" s="5"/>
       <c r="W199" s="5"/>
@@ -7869,14 +8258,14 @@
       <c r="A200" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B200" s="96" t="s">
+      <c r="B200" s="97" t="s">
         <v>288</v>
       </c>
-      <c r="C200" s="97"/>
-      <c r="D200" s="96" t="s">
+      <c r="C200" s="96"/>
+      <c r="D200" s="97" t="s">
         <v>289</v>
       </c>
-      <c r="E200" s="97"/>
+      <c r="E200" s="96"/>
       <c r="F200" s="62" t="s">
         <v>290</v>
       </c>
@@ -7890,14 +8279,14 @@
       <c r="A201" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B201" s="99" t="s">
+      <c r="B201" s="95" t="s">
         <v>291</v>
       </c>
-      <c r="C201" s="97"/>
-      <c r="D201" s="99" t="s">
+      <c r="C201" s="96"/>
+      <c r="D201" s="95" t="s">
         <v>292</v>
       </c>
-      <c r="E201" s="97"/>
+      <c r="E201" s="96"/>
       <c r="F201" s="63" t="s">
         <v>293</v>
       </c>
@@ -7914,14 +8303,14 @@
       <c r="A202" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B202" s="96" t="s">
+      <c r="B202" s="97" t="s">
         <v>294</v>
       </c>
-      <c r="C202" s="97"/>
-      <c r="D202" s="96" t="s">
+      <c r="C202" s="96"/>
+      <c r="D202" s="97" t="s">
         <v>295</v>
       </c>
-      <c r="E202" s="97"/>
+      <c r="E202" s="96"/>
       <c r="F202" s="62" t="s">
         <v>296</v>
       </c>
@@ -7945,14 +8334,14 @@
       <c r="A203" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B203" s="99" t="s">
+      <c r="B203" s="95" t="s">
         <v>297</v>
       </c>
-      <c r="C203" s="97"/>
-      <c r="D203" s="99" t="s">
+      <c r="C203" s="96"/>
+      <c r="D203" s="95" t="s">
         <v>298</v>
       </c>
-      <c r="E203" s="97"/>
+      <c r="E203" s="96"/>
       <c r="F203" s="63" t="s">
         <v>299</v>
       </c>
@@ -7975,14 +8364,14 @@
       <c r="A204" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B204" s="96" t="s">
+      <c r="B204" s="97" t="s">
         <v>290</v>
       </c>
-      <c r="C204" s="97"/>
-      <c r="D204" s="96" t="s">
+      <c r="C204" s="96"/>
+      <c r="D204" s="97" t="s">
         <v>300</v>
       </c>
-      <c r="E204" s="97"/>
+      <c r="E204" s="96"/>
       <c r="F204" s="62" t="s">
         <v>301</v>
       </c>
@@ -8005,14 +8394,14 @@
       <c r="A205" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B205" s="99" t="s">
+      <c r="B205" s="95" t="s">
         <v>302</v>
       </c>
-      <c r="C205" s="97"/>
-      <c r="D205" s="99" t="s">
+      <c r="C205" s="96"/>
+      <c r="D205" s="95" t="s">
         <v>303</v>
       </c>
-      <c r="E205" s="97"/>
+      <c r="E205" s="96"/>
       <c r="F205" s="63" t="s">
         <v>304</v>
       </c>
@@ -8035,14 +8424,14 @@
       <c r="A206" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B206" s="96" t="s">
+      <c r="B206" s="97" t="s">
         <v>305</v>
       </c>
-      <c r="C206" s="97"/>
-      <c r="D206" s="96" t="s">
+      <c r="C206" s="96"/>
+      <c r="D206" s="97" t="s">
         <v>306</v>
       </c>
-      <c r="E206" s="97"/>
+      <c r="E206" s="96"/>
       <c r="F206" s="62" t="s">
         <v>307</v>
       </c>
@@ -8065,14 +8454,14 @@
       <c r="A207" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B207" s="99" t="s">
+      <c r="B207" s="95" t="s">
         <v>308</v>
       </c>
-      <c r="C207" s="97"/>
-      <c r="D207" s="99" t="s">
+      <c r="C207" s="96"/>
+      <c r="D207" s="95" t="s">
         <v>309</v>
       </c>
-      <c r="E207" s="97"/>
+      <c r="E207" s="96"/>
       <c r="F207" s="63" t="s">
         <v>310</v>
       </c>
@@ -8096,14 +8485,14 @@
       <c r="A208" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B208" s="96" t="s">
+      <c r="B208" s="97" t="s">
         <v>311</v>
       </c>
-      <c r="C208" s="97"/>
-      <c r="D208" s="96" t="s">
+      <c r="C208" s="96"/>
+      <c r="D208" s="97" t="s">
         <v>312</v>
       </c>
-      <c r="E208" s="97"/>
+      <c r="E208" s="96"/>
       <c r="F208" s="62" t="s">
         <v>313</v>
       </c>
@@ -8127,14 +8516,14 @@
       <c r="A209" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B209" s="115">
+      <c r="B209" s="104">
         <v>7.65</v>
       </c>
-      <c r="C209" s="97"/>
-      <c r="D209" s="99" t="s">
+      <c r="C209" s="96"/>
+      <c r="D209" s="95" t="s">
         <v>314</v>
       </c>
-      <c r="E209" s="97"/>
+      <c r="E209" s="96"/>
       <c r="F209" s="63" t="s">
         <v>315</v>
       </c>
@@ -8158,14 +8547,14 @@
       <c r="A210" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B210" s="96" t="s">
+      <c r="B210" s="97" t="s">
         <v>316</v>
       </c>
-      <c r="C210" s="97"/>
-      <c r="D210" s="96" t="s">
+      <c r="C210" s="96"/>
+      <c r="D210" s="97" t="s">
         <v>317</v>
       </c>
-      <c r="E210" s="97"/>
+      <c r="E210" s="96"/>
       <c r="F210" s="62" t="s">
         <v>300</v>
       </c>
@@ -8188,14 +8577,14 @@
       <c r="A211" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B211" s="115">
+      <c r="B211" s="104">
         <v>7.71</v>
       </c>
-      <c r="C211" s="97"/>
-      <c r="D211" s="99" t="s">
+      <c r="C211" s="96"/>
+      <c r="D211" s="95" t="s">
         <v>318</v>
       </c>
-      <c r="E211" s="97"/>
+      <c r="E211" s="96"/>
       <c r="F211" s="63" t="s">
         <v>319</v>
       </c>
@@ -8219,14 +8608,14 @@
       <c r="A212" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B212" s="96" t="s">
+      <c r="B212" s="97" t="s">
         <v>320</v>
       </c>
-      <c r="C212" s="97"/>
-      <c r="D212" s="96" t="s">
+      <c r="C212" s="96"/>
+      <c r="D212" s="97" t="s">
         <v>321</v>
       </c>
-      <c r="E212" s="97"/>
+      <c r="E212" s="96"/>
       <c r="F212" s="62" t="s">
         <v>322</v>
       </c>
@@ -8249,14 +8638,14 @@
       <c r="A213" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B213" s="115">
+      <c r="B213" s="104">
         <v>7.77</v>
       </c>
-      <c r="C213" s="97"/>
-      <c r="D213" s="99" t="s">
+      <c r="C213" s="96"/>
+      <c r="D213" s="95" t="s">
         <v>323</v>
       </c>
-      <c r="E213" s="97"/>
+      <c r="E213" s="96"/>
       <c r="F213" s="63" t="s">
         <v>314</v>
       </c>
@@ -8280,14 +8669,14 @@
       <c r="A214" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B214" s="96" t="s">
+      <c r="B214" s="97" t="s">
         <v>307</v>
       </c>
-      <c r="C214" s="97"/>
-      <c r="D214" s="96" t="s">
+      <c r="C214" s="96"/>
+      <c r="D214" s="97" t="s">
         <v>324</v>
       </c>
-      <c r="E214" s="97"/>
+      <c r="E214" s="96"/>
       <c r="F214" s="62" t="s">
         <v>325</v>
       </c>
@@ -8311,14 +8700,14 @@
       <c r="A215" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B215" s="115">
+      <c r="B215" s="104">
         <v>7.83</v>
       </c>
-      <c r="C215" s="97"/>
-      <c r="D215" s="99" t="s">
+      <c r="C215" s="96"/>
+      <c r="D215" s="95" t="s">
         <v>326</v>
       </c>
-      <c r="E215" s="97"/>
+      <c r="E215" s="96"/>
       <c r="F215" s="63" t="s">
         <v>327</v>
       </c>
@@ -8342,14 +8731,14 @@
       <c r="A216" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B216" s="96" t="s">
+      <c r="B216" s="97" t="s">
         <v>328</v>
       </c>
-      <c r="C216" s="97"/>
-      <c r="D216" s="96" t="s">
+      <c r="C216" s="96"/>
+      <c r="D216" s="97" t="s">
         <v>329</v>
       </c>
-      <c r="E216" s="97"/>
+      <c r="E216" s="96"/>
       <c r="F216" s="62" t="s">
         <v>324</v>
       </c>
@@ -8373,14 +8762,14 @@
       <c r="A217" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B217" s="115">
+      <c r="B217" s="104">
         <v>7.89</v>
       </c>
-      <c r="C217" s="97"/>
-      <c r="D217" s="99" t="s">
+      <c r="C217" s="96"/>
+      <c r="D217" s="95" t="s">
         <v>330</v>
       </c>
-      <c r="E217" s="97"/>
+      <c r="E217" s="96"/>
       <c r="F217" s="63" t="s">
         <v>331</v>
       </c>
@@ -8401,14 +8790,14 @@
       <c r="A218" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B218" s="96" t="s">
+      <c r="B218" s="97" t="s">
         <v>332</v>
       </c>
-      <c r="C218" s="97"/>
-      <c r="D218" s="96" t="s">
+      <c r="C218" s="96"/>
+      <c r="D218" s="97" t="s">
         <v>333</v>
       </c>
-      <c r="E218" s="97"/>
+      <c r="E218" s="96"/>
       <c r="F218" s="62" t="s">
         <v>334</v>
       </c>
@@ -8429,14 +8818,14 @@
       <c r="A219" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="B219" s="116">
+      <c r="B219" s="109">
         <v>7.95</v>
       </c>
-      <c r="C219" s="103"/>
-      <c r="D219" s="102" t="s">
+      <c r="C219" s="101"/>
+      <c r="D219" s="100" t="s">
         <v>335</v>
       </c>
-      <c r="E219" s="103"/>
+      <c r="E219" s="101"/>
       <c r="F219" s="66" t="s">
         <v>335</v>
       </c>
@@ -8866,21 +9255,21 @@
       <c r="A251" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B251" s="93" t="s">
+      <c r="B251" s="103" t="s">
         <v>368</v>
       </c>
-      <c r="C251" s="94"/>
-      <c r="D251" s="94"/>
-      <c r="E251" s="93" t="s">
+      <c r="C251" s="99"/>
+      <c r="D251" s="99"/>
+      <c r="E251" s="103" t="s">
         <v>369</v>
       </c>
-      <c r="F251" s="94"/>
-      <c r="G251" s="94"/>
-      <c r="H251" s="93" t="s">
+      <c r="F251" s="99"/>
+      <c r="G251" s="99"/>
+      <c r="H251" s="103" t="s">
         <v>370</v>
       </c>
-      <c r="I251" s="94"/>
-      <c r="J251" s="95"/>
+      <c r="I251" s="99"/>
+      <c r="J251" s="116"/>
       <c r="P251" s="5"/>
       <c r="Q251" s="5"/>
       <c r="R251" s="12"/>
@@ -8891,21 +9280,21 @@
       <c r="A252" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B252" s="96" t="s">
+      <c r="B252" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="C252" s="97"/>
-      <c r="D252" s="97"/>
-      <c r="E252" s="96" t="s">
+      <c r="C252" s="96"/>
+      <c r="D252" s="96"/>
+      <c r="E252" s="97" t="s">
         <v>18</v>
       </c>
-      <c r="F252" s="97"/>
-      <c r="G252" s="97"/>
-      <c r="H252" s="96" t="s">
+      <c r="F252" s="96"/>
+      <c r="G252" s="96"/>
+      <c r="H252" s="97" t="s">
         <v>371</v>
       </c>
-      <c r="I252" s="97"/>
-      <c r="J252" s="98"/>
+      <c r="I252" s="96"/>
+      <c r="J252" s="105"/>
       <c r="P252" s="5"/>
       <c r="Q252" s="5"/>
       <c r="R252" s="12"/>
@@ -8916,21 +9305,21 @@
       <c r="A253" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B253" s="99" t="s">
+      <c r="B253" s="95" t="s">
         <v>18</v>
       </c>
-      <c r="C253" s="97"/>
-      <c r="D253" s="97"/>
-      <c r="E253" s="99" t="s">
+      <c r="C253" s="96"/>
+      <c r="D253" s="96"/>
+      <c r="E253" s="95" t="s">
         <v>372</v>
       </c>
-      <c r="F253" s="97"/>
-      <c r="G253" s="97"/>
-      <c r="H253" s="99" t="s">
+      <c r="F253" s="96"/>
+      <c r="G253" s="96"/>
+      <c r="H253" s="95" t="s">
         <v>371</v>
       </c>
-      <c r="I253" s="97"/>
-      <c r="J253" s="98"/>
+      <c r="I253" s="96"/>
+      <c r="J253" s="105"/>
       <c r="P253" s="5"/>
       <c r="Q253" s="5"/>
       <c r="R253" s="12"/>
@@ -8941,21 +9330,21 @@
       <c r="A254" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B254" s="96" t="s">
+      <c r="B254" s="97" t="s">
         <v>373</v>
       </c>
-      <c r="C254" s="97"/>
-      <c r="D254" s="97"/>
-      <c r="E254" s="96" t="s">
+      <c r="C254" s="96"/>
+      <c r="D254" s="96"/>
+      <c r="E254" s="97" t="s">
         <v>373</v>
       </c>
-      <c r="F254" s="97"/>
-      <c r="G254" s="97"/>
-      <c r="H254" s="96" t="s">
+      <c r="F254" s="96"/>
+      <c r="G254" s="96"/>
+      <c r="H254" s="97" t="s">
         <v>371</v>
       </c>
-      <c r="I254" s="97"/>
-      <c r="J254" s="98"/>
+      <c r="I254" s="96"/>
+      <c r="J254" s="105"/>
       <c r="P254" s="5"/>
       <c r="Q254" s="5"/>
       <c r="R254" s="12"/>
@@ -8966,21 +9355,21 @@
       <c r="A255" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B255" s="99" t="s">
+      <c r="B255" s="95" t="s">
         <v>373</v>
       </c>
-      <c r="C255" s="97"/>
-      <c r="D255" s="97"/>
-      <c r="E255" s="99" t="s">
+      <c r="C255" s="96"/>
+      <c r="D255" s="96"/>
+      <c r="E255" s="95" t="s">
         <v>374</v>
       </c>
-      <c r="F255" s="97"/>
-      <c r="G255" s="97"/>
-      <c r="H255" s="99" t="s">
+      <c r="F255" s="96"/>
+      <c r="G255" s="96"/>
+      <c r="H255" s="95" t="s">
         <v>371</v>
       </c>
-      <c r="I255" s="97"/>
-      <c r="J255" s="98"/>
+      <c r="I255" s="96"/>
+      <c r="J255" s="105"/>
       <c r="P255" s="5"/>
       <c r="Q255" s="5"/>
       <c r="R255" s="12"/>
@@ -8991,21 +9380,21 @@
       <c r="A256" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B256" s="96" t="s">
+      <c r="B256" s="97" t="s">
         <v>375</v>
       </c>
-      <c r="C256" s="97"/>
-      <c r="D256" s="97"/>
-      <c r="E256" s="96" t="s">
+      <c r="C256" s="96"/>
+      <c r="D256" s="96"/>
+      <c r="E256" s="97" t="s">
         <v>376</v>
       </c>
-      <c r="F256" s="97"/>
-      <c r="G256" s="97"/>
-      <c r="H256" s="96" t="s">
+      <c r="F256" s="96"/>
+      <c r="G256" s="96"/>
+      <c r="H256" s="97" t="s">
         <v>377</v>
       </c>
-      <c r="I256" s="97"/>
-      <c r="J256" s="98"/>
+      <c r="I256" s="96"/>
+      <c r="J256" s="105"/>
       <c r="P256" s="5"/>
       <c r="Q256" s="5"/>
       <c r="R256" s="12"/>
@@ -9016,21 +9405,21 @@
       <c r="A257" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B257" s="99" t="s">
+      <c r="B257" s="95" t="s">
         <v>375</v>
       </c>
-      <c r="C257" s="97"/>
-      <c r="D257" s="97"/>
-      <c r="E257" s="99" t="s">
+      <c r="C257" s="96"/>
+      <c r="D257" s="96"/>
+      <c r="E257" s="95" t="s">
         <v>378</v>
       </c>
-      <c r="F257" s="97"/>
-      <c r="G257" s="97"/>
-      <c r="H257" s="99" t="s">
+      <c r="F257" s="96"/>
+      <c r="G257" s="96"/>
+      <c r="H257" s="95" t="s">
         <v>377</v>
       </c>
-      <c r="I257" s="97"/>
-      <c r="J257" s="98"/>
+      <c r="I257" s="96"/>
+      <c r="J257" s="105"/>
       <c r="P257" s="5"/>
       <c r="Q257" s="5"/>
       <c r="R257" s="12"/>
@@ -9041,21 +9430,21 @@
       <c r="A258" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B258" s="96" t="s">
+      <c r="B258" s="97" t="s">
         <v>379</v>
       </c>
-      <c r="C258" s="97"/>
-      <c r="D258" s="97"/>
-      <c r="E258" s="96" t="s">
+      <c r="C258" s="96"/>
+      <c r="D258" s="96"/>
+      <c r="E258" s="97" t="s">
         <v>380</v>
       </c>
-      <c r="F258" s="97"/>
-      <c r="G258" s="97"/>
-      <c r="H258" s="96" t="s">
+      <c r="F258" s="96"/>
+      <c r="G258" s="96"/>
+      <c r="H258" s="97" t="s">
         <v>377</v>
       </c>
-      <c r="I258" s="97"/>
-      <c r="J258" s="98"/>
+      <c r="I258" s="96"/>
+      <c r="J258" s="105"/>
       <c r="K258" s="5"/>
       <c r="P258" s="5"/>
       <c r="Q258" s="5"/>
@@ -9067,21 +9456,21 @@
       <c r="A259" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B259" s="99" t="s">
+      <c r="B259" s="95" t="s">
         <v>379</v>
       </c>
-      <c r="C259" s="97"/>
-      <c r="D259" s="97"/>
-      <c r="E259" s="99" t="s">
+      <c r="C259" s="96"/>
+      <c r="D259" s="96"/>
+      <c r="E259" s="95" t="s">
         <v>381</v>
       </c>
-      <c r="F259" s="97"/>
-      <c r="G259" s="97"/>
-      <c r="H259" s="99" t="s">
+      <c r="F259" s="96"/>
+      <c r="G259" s="96"/>
+      <c r="H259" s="95" t="s">
         <v>377</v>
       </c>
-      <c r="I259" s="97"/>
-      <c r="J259" s="98"/>
+      <c r="I259" s="96"/>
+      <c r="J259" s="105"/>
       <c r="K259" s="5"/>
       <c r="P259" s="5"/>
       <c r="Q259" s="5"/>
@@ -9093,21 +9482,21 @@
       <c r="A260" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B260" s="96" t="s">
+      <c r="B260" s="97" t="s">
         <v>380</v>
       </c>
-      <c r="C260" s="97"/>
-      <c r="D260" s="97"/>
-      <c r="E260" s="96" t="s">
+      <c r="C260" s="96"/>
+      <c r="D260" s="96"/>
+      <c r="E260" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="F260" s="97"/>
-      <c r="G260" s="97"/>
-      <c r="H260" s="96" t="s">
+      <c r="F260" s="96"/>
+      <c r="G260" s="96"/>
+      <c r="H260" s="97" t="s">
         <v>383</v>
       </c>
-      <c r="I260" s="97"/>
-      <c r="J260" s="98"/>
+      <c r="I260" s="96"/>
+      <c r="J260" s="105"/>
       <c r="K260" s="5"/>
       <c r="P260" s="5"/>
       <c r="Q260" s="5"/>
@@ -9118,21 +9507,21 @@
       <c r="A261" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B261" s="99" t="s">
+      <c r="B261" s="95" t="s">
         <v>381</v>
       </c>
-      <c r="C261" s="97"/>
-      <c r="D261" s="97"/>
-      <c r="E261" s="99" t="s">
+      <c r="C261" s="96"/>
+      <c r="D261" s="96"/>
+      <c r="E261" s="95" t="s">
         <v>384</v>
       </c>
-      <c r="F261" s="97"/>
-      <c r="G261" s="97"/>
-      <c r="H261" s="99" t="s">
+      <c r="F261" s="96"/>
+      <c r="G261" s="96"/>
+      <c r="H261" s="95" t="s">
         <v>383</v>
       </c>
-      <c r="I261" s="97"/>
-      <c r="J261" s="98"/>
+      <c r="I261" s="96"/>
+      <c r="J261" s="105"/>
       <c r="K261" s="5"/>
       <c r="P261" s="5"/>
       <c r="Q261" s="5"/>
@@ -9144,21 +9533,21 @@
       <c r="A262" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B262" s="96" t="s">
+      <c r="B262" s="97" t="s">
         <v>385</v>
       </c>
-      <c r="C262" s="97"/>
-      <c r="D262" s="97"/>
-      <c r="E262" s="96" t="s">
+      <c r="C262" s="96"/>
+      <c r="D262" s="96"/>
+      <c r="E262" s="97" t="s">
         <v>386</v>
       </c>
-      <c r="F262" s="97"/>
-      <c r="G262" s="97"/>
-      <c r="H262" s="96" t="s">
+      <c r="F262" s="96"/>
+      <c r="G262" s="96"/>
+      <c r="H262" s="97" t="s">
         <v>383</v>
       </c>
-      <c r="I262" s="97"/>
-      <c r="J262" s="98"/>
+      <c r="I262" s="96"/>
+      <c r="J262" s="105"/>
       <c r="K262" s="5"/>
       <c r="P262" s="5"/>
       <c r="Q262" s="5"/>
@@ -9170,21 +9559,21 @@
       <c r="A263" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B263" s="99" t="s">
+      <c r="B263" s="95" t="s">
         <v>387</v>
       </c>
-      <c r="C263" s="97"/>
-      <c r="D263" s="97"/>
-      <c r="E263" s="99" t="s">
+      <c r="C263" s="96"/>
+      <c r="D263" s="96"/>
+      <c r="E263" s="95" t="s">
         <v>388</v>
       </c>
-      <c r="F263" s="97"/>
-      <c r="G263" s="97"/>
-      <c r="H263" s="99" t="s">
+      <c r="F263" s="96"/>
+      <c r="G263" s="96"/>
+      <c r="H263" s="95" t="s">
         <v>383</v>
       </c>
-      <c r="I263" s="97"/>
-      <c r="J263" s="98"/>
+      <c r="I263" s="96"/>
+      <c r="J263" s="105"/>
       <c r="K263" s="5"/>
       <c r="P263" s="5"/>
       <c r="Q263" s="5"/>
@@ -9196,21 +9585,21 @@
       <c r="A264" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B264" s="96" t="s">
+      <c r="B264" s="97" t="s">
         <v>382</v>
       </c>
-      <c r="C264" s="97"/>
-      <c r="D264" s="97"/>
-      <c r="E264" s="96" t="s">
+      <c r="C264" s="96"/>
+      <c r="D264" s="96"/>
+      <c r="E264" s="97" t="s">
         <v>389</v>
       </c>
-      <c r="F264" s="97"/>
-      <c r="G264" s="97"/>
-      <c r="H264" s="96" t="s">
+      <c r="F264" s="96"/>
+      <c r="G264" s="96"/>
+      <c r="H264" s="97" t="s">
         <v>390</v>
       </c>
-      <c r="I264" s="97"/>
-      <c r="J264" s="98"/>
+      <c r="I264" s="96"/>
+      <c r="J264" s="105"/>
       <c r="K264" s="5"/>
       <c r="P264" s="5"/>
       <c r="Q264" s="5"/>
@@ -9222,21 +9611,21 @@
       <c r="A265" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B265" s="99" t="s">
+      <c r="B265" s="95" t="s">
         <v>384</v>
       </c>
-      <c r="C265" s="97"/>
-      <c r="D265" s="97"/>
-      <c r="E265" s="99" t="s">
+      <c r="C265" s="96"/>
+      <c r="D265" s="96"/>
+      <c r="E265" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="F265" s="97"/>
-      <c r="G265" s="97"/>
-      <c r="H265" s="99" t="s">
+      <c r="F265" s="96"/>
+      <c r="G265" s="96"/>
+      <c r="H265" s="95" t="s">
         <v>390</v>
       </c>
-      <c r="I265" s="97"/>
-      <c r="J265" s="98"/>
+      <c r="I265" s="96"/>
+      <c r="J265" s="105"/>
       <c r="K265" s="5"/>
       <c r="P265" s="5"/>
       <c r="Q265" s="5"/>
@@ -9248,21 +9637,21 @@
       <c r="A266" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B266" s="96" t="s">
+      <c r="B266" s="97" t="s">
         <v>386</v>
       </c>
-      <c r="C266" s="97"/>
-      <c r="D266" s="97"/>
-      <c r="E266" s="96" t="s">
+      <c r="C266" s="96"/>
+      <c r="D266" s="96"/>
+      <c r="E266" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="F266" s="97"/>
-      <c r="G266" s="97"/>
-      <c r="H266" s="96" t="s">
+      <c r="F266" s="96"/>
+      <c r="G266" s="96"/>
+      <c r="H266" s="97" t="s">
         <v>390</v>
       </c>
-      <c r="I266" s="97"/>
-      <c r="J266" s="98"/>
+      <c r="I266" s="96"/>
+      <c r="J266" s="105"/>
       <c r="K266" s="5"/>
       <c r="P266" s="5"/>
       <c r="Q266" s="5"/>
@@ -9279,21 +9668,21 @@
       <c r="A267" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B267" s="99" t="s">
+      <c r="B267" s="95" t="s">
         <v>388</v>
       </c>
-      <c r="C267" s="97"/>
-      <c r="D267" s="97"/>
-      <c r="E267" s="99" t="s">
+      <c r="C267" s="96"/>
+      <c r="D267" s="96"/>
+      <c r="E267" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="F267" s="97"/>
-      <c r="G267" s="97"/>
-      <c r="H267" s="99" t="s">
+      <c r="F267" s="96"/>
+      <c r="G267" s="96"/>
+      <c r="H267" s="95" t="s">
         <v>390</v>
       </c>
-      <c r="I267" s="97"/>
-      <c r="J267" s="98"/>
+      <c r="I267" s="96"/>
+      <c r="J267" s="105"/>
       <c r="K267" s="5"/>
       <c r="P267" s="5"/>
       <c r="Q267" s="5"/>
@@ -9310,21 +9699,21 @@
       <c r="A268" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B268" s="96" t="s">
+      <c r="B268" s="97" t="s">
         <v>389</v>
       </c>
-      <c r="C268" s="97"/>
-      <c r="D268" s="97"/>
-      <c r="E268" s="96" t="s">
+      <c r="C268" s="96"/>
+      <c r="D268" s="96"/>
+      <c r="E268" s="97" t="s">
         <v>206</v>
       </c>
-      <c r="F268" s="97"/>
-      <c r="G268" s="97"/>
-      <c r="H268" s="96" t="s">
+      <c r="F268" s="96"/>
+      <c r="G268" s="96"/>
+      <c r="H268" s="97" t="s">
         <v>191</v>
       </c>
-      <c r="I268" s="97"/>
-      <c r="J268" s="98"/>
+      <c r="I268" s="96"/>
+      <c r="J268" s="105"/>
       <c r="K268" s="5"/>
       <c r="P268" s="5"/>
       <c r="Q268" s="5"/>
@@ -9339,21 +9728,21 @@
       <c r="A269" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B269" s="99" t="s">
+      <c r="B269" s="95" t="s">
         <v>194</v>
       </c>
-      <c r="C269" s="97"/>
-      <c r="D269" s="97"/>
-      <c r="E269" s="99" t="s">
+      <c r="C269" s="96"/>
+      <c r="D269" s="96"/>
+      <c r="E269" s="95" t="s">
         <v>391</v>
       </c>
-      <c r="F269" s="97"/>
-      <c r="G269" s="97"/>
-      <c r="H269" s="99" t="s">
+      <c r="F269" s="96"/>
+      <c r="G269" s="96"/>
+      <c r="H269" s="95" t="s">
         <v>191</v>
       </c>
-      <c r="I269" s="97"/>
-      <c r="J269" s="98"/>
+      <c r="I269" s="96"/>
+      <c r="J269" s="105"/>
       <c r="K269" s="5"/>
       <c r="P269" s="5"/>
       <c r="Q269" s="5"/>
@@ -9367,21 +9756,21 @@
       <c r="A270" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B270" s="96" t="s">
+      <c r="B270" s="97" t="s">
         <v>188</v>
       </c>
-      <c r="C270" s="97"/>
-      <c r="D270" s="97"/>
-      <c r="E270" s="96" t="s">
+      <c r="C270" s="96"/>
+      <c r="D270" s="96"/>
+      <c r="E270" s="97" t="s">
         <v>392</v>
       </c>
-      <c r="F270" s="97"/>
-      <c r="G270" s="97"/>
-      <c r="H270" s="96" t="s">
+      <c r="F270" s="96"/>
+      <c r="G270" s="96"/>
+      <c r="H270" s="97" t="s">
         <v>191</v>
       </c>
-      <c r="I270" s="97"/>
-      <c r="J270" s="98"/>
+      <c r="I270" s="96"/>
+      <c r="J270" s="105"/>
       <c r="K270" s="5"/>
       <c r="P270" s="5"/>
       <c r="Q270" s="5"/>
@@ -9397,21 +9786,21 @@
       <c r="A271" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="B271" s="102" t="s">
+      <c r="B271" s="100" t="s">
         <v>179</v>
       </c>
-      <c r="C271" s="103"/>
-      <c r="D271" s="103"/>
-      <c r="E271" s="102" t="s">
+      <c r="C271" s="101"/>
+      <c r="D271" s="101"/>
+      <c r="E271" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="F271" s="103"/>
-      <c r="G271" s="103"/>
-      <c r="H271" s="102" t="s">
+      <c r="F271" s="101"/>
+      <c r="G271" s="101"/>
+      <c r="H271" s="100" t="s">
         <v>191</v>
       </c>
-      <c r="I271" s="103"/>
-      <c r="J271" s="105"/>
+      <c r="I271" s="101"/>
+      <c r="J271" s="117"/>
       <c r="K271" s="5"/>
       <c r="O271" s="5"/>
       <c r="P271" s="5"/>
@@ -9495,23 +9884,23 @@
       <c r="Z276" s="5"/>
     </row>
     <row r="277" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A277" s="106" t="s">
+      <c r="A277" s="110" t="s">
         <v>4</v>
       </c>
-      <c r="B277" s="104" t="s">
+      <c r="B277" s="102" t="s">
         <v>395</v>
       </c>
-      <c r="C277" s="94"/>
-      <c r="D277" s="94"/>
-      <c r="E277" s="100" t="s">
+      <c r="C277" s="99"/>
+      <c r="D277" s="99"/>
+      <c r="E277" s="118" t="s">
         <v>9</v>
       </c>
-      <c r="F277" s="94"/>
-      <c r="G277" s="94"/>
-      <c r="H277" s="104" t="s">
+      <c r="F277" s="99"/>
+      <c r="G277" s="99"/>
+      <c r="H277" s="102" t="s">
         <v>10</v>
       </c>
-      <c r="I277" s="95"/>
+      <c r="I277" s="116"/>
       <c r="J277" s="5"/>
       <c r="K277" s="5"/>
       <c r="P277" s="5"/>
@@ -9526,7 +9915,7 @@
       <c r="Z277" s="5"/>
     </row>
     <row r="278" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A278" s="107"/>
+      <c r="A278" s="111"/>
       <c r="B278" s="68" t="s">
         <v>339</v>
       </c>
@@ -10466,24 +10855,24 @@
       <c r="Z303" s="5"/>
     </row>
     <row r="304" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A304" s="106" t="s">
+      <c r="A304" s="110" t="s">
         <v>5</v>
       </c>
-      <c r="B304" s="117" t="s">
+      <c r="B304" s="98" t="s">
         <v>502</v>
       </c>
-      <c r="C304" s="94"/>
-      <c r="D304" s="94"/>
-      <c r="E304" s="100" t="s">
+      <c r="C304" s="99"/>
+      <c r="D304" s="99"/>
+      <c r="E304" s="118" t="s">
         <v>503</v>
       </c>
-      <c r="F304" s="94"/>
-      <c r="G304" s="94"/>
-      <c r="H304" s="101" t="s">
+      <c r="F304" s="99"/>
+      <c r="G304" s="99"/>
+      <c r="H304" s="119" t="s">
         <v>504</v>
       </c>
-      <c r="I304" s="94"/>
-      <c r="J304" s="95"/>
+      <c r="I304" s="99"/>
+      <c r="J304" s="116"/>
       <c r="K304" s="75"/>
       <c r="L304" s="75"/>
       <c r="M304" s="75"/>
@@ -10502,7 +10891,7 @@
       <c r="Z304" s="5"/>
     </row>
     <row r="305" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A305" s="107"/>
+      <c r="A305" s="111"/>
       <c r="B305" s="68" t="s">
         <v>339</v>
       </c>
@@ -11546,16 +11935,16 @@
       <c r="A331" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B331" s="93" t="s">
+      <c r="B331" s="103" t="s">
         <v>210</v>
       </c>
-      <c r="C331" s="94"/>
-      <c r="D331" s="94"/>
-      <c r="E331" s="93" t="s">
+      <c r="C331" s="99"/>
+      <c r="D331" s="99"/>
+      <c r="E331" s="103" t="s">
         <v>211</v>
       </c>
-      <c r="F331" s="94"/>
-      <c r="G331" s="95"/>
+      <c r="F331" s="99"/>
+      <c r="G331" s="116"/>
       <c r="H331" s="5"/>
       <c r="O331" s="5"/>
       <c r="P331" s="5"/>
@@ -11574,16 +11963,16 @@
       <c r="A332" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="B332" s="96" t="s">
+      <c r="B332" s="97" t="s">
         <v>577</v>
       </c>
-      <c r="C332" s="97"/>
-      <c r="D332" s="97"/>
-      <c r="E332" s="96" t="s">
+      <c r="C332" s="96"/>
+      <c r="D332" s="96"/>
+      <c r="E332" s="97" t="s">
         <v>578</v>
       </c>
-      <c r="F332" s="97"/>
-      <c r="G332" s="98"/>
+      <c r="F332" s="96"/>
+      <c r="G332" s="105"/>
       <c r="H332" s="5"/>
       <c r="O332" s="5"/>
       <c r="P332" s="5"/>
@@ -11602,16 +11991,16 @@
       <c r="A333" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="B333" s="99" t="s">
+      <c r="B333" s="95" t="s">
         <v>577</v>
       </c>
-      <c r="C333" s="97"/>
-      <c r="D333" s="97"/>
-      <c r="E333" s="99" t="s">
+      <c r="C333" s="96"/>
+      <c r="D333" s="96"/>
+      <c r="E333" s="95" t="s">
         <v>390</v>
       </c>
-      <c r="F333" s="97"/>
-      <c r="G333" s="98"/>
+      <c r="F333" s="96"/>
+      <c r="G333" s="105"/>
       <c r="H333" s="5"/>
       <c r="O333" s="5"/>
       <c r="P333" s="5"/>
@@ -11630,16 +12019,16 @@
       <c r="A334" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B334" s="96" t="s">
+      <c r="B334" s="97" t="s">
         <v>579</v>
       </c>
-      <c r="C334" s="97"/>
-      <c r="D334" s="97"/>
-      <c r="E334" s="96" t="s">
+      <c r="C334" s="96"/>
+      <c r="D334" s="96"/>
+      <c r="E334" s="97" t="s">
         <v>580</v>
       </c>
-      <c r="F334" s="97"/>
-      <c r="G334" s="98"/>
+      <c r="F334" s="96"/>
+      <c r="G334" s="105"/>
       <c r="H334" s="5"/>
       <c r="O334" s="5"/>
       <c r="P334" s="5"/>
@@ -11658,16 +12047,16 @@
       <c r="A335" s="14" t="s">
         <v>152</v>
       </c>
-      <c r="B335" s="99" t="s">
+      <c r="B335" s="95" t="s">
         <v>579</v>
       </c>
-      <c r="C335" s="97"/>
-      <c r="D335" s="97"/>
-      <c r="E335" s="99" t="s">
+      <c r="C335" s="96"/>
+      <c r="D335" s="96"/>
+      <c r="E335" s="95" t="s">
         <v>214</v>
       </c>
-      <c r="F335" s="97"/>
-      <c r="G335" s="98"/>
+      <c r="F335" s="96"/>
+      <c r="G335" s="105"/>
       <c r="H335" s="5"/>
       <c r="O335" s="5"/>
       <c r="P335" s="5"/>
@@ -11686,16 +12075,16 @@
       <c r="A336" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B336" s="96" t="s">
+      <c r="B336" s="97" t="s">
         <v>213</v>
       </c>
-      <c r="C336" s="97"/>
-      <c r="D336" s="97"/>
-      <c r="E336" s="96" t="s">
+      <c r="C336" s="96"/>
+      <c r="D336" s="96"/>
+      <c r="E336" s="97" t="s">
         <v>581</v>
       </c>
-      <c r="F336" s="97"/>
-      <c r="G336" s="98"/>
+      <c r="F336" s="96"/>
+      <c r="G336" s="105"/>
       <c r="H336" s="5"/>
       <c r="O336" s="5"/>
       <c r="P336" s="5"/>
@@ -11714,16 +12103,16 @@
       <c r="A337" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B337" s="99" t="s">
+      <c r="B337" s="95" t="s">
         <v>213</v>
       </c>
-      <c r="C337" s="97"/>
-      <c r="D337" s="97"/>
-      <c r="E337" s="99" t="s">
+      <c r="C337" s="96"/>
+      <c r="D337" s="96"/>
+      <c r="E337" s="95" t="s">
         <v>582</v>
       </c>
-      <c r="F337" s="97"/>
-      <c r="G337" s="98"/>
+      <c r="F337" s="96"/>
+      <c r="G337" s="105"/>
       <c r="H337" s="5"/>
       <c r="O337" s="5"/>
       <c r="P337" s="5"/>
@@ -11742,16 +12131,16 @@
       <c r="A338" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B338" s="96" t="s">
+      <c r="B338" s="97" t="s">
         <v>583</v>
       </c>
-      <c r="C338" s="97"/>
-      <c r="D338" s="97"/>
-      <c r="E338" s="96" t="s">
+      <c r="C338" s="96"/>
+      <c r="D338" s="96"/>
+      <c r="E338" s="97" t="s">
         <v>584</v>
       </c>
-      <c r="F338" s="97"/>
-      <c r="G338" s="98"/>
+      <c r="F338" s="96"/>
+      <c r="G338" s="105"/>
       <c r="H338" s="5"/>
       <c r="O338" s="5"/>
       <c r="P338" s="5"/>
@@ -11770,16 +12159,16 @@
       <c r="A339" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="B339" s="99" t="s">
+      <c r="B339" s="95" t="s">
         <v>583</v>
       </c>
-      <c r="C339" s="97"/>
-      <c r="D339" s="97"/>
-      <c r="E339" s="99" t="s">
+      <c r="C339" s="96"/>
+      <c r="D339" s="96"/>
+      <c r="E339" s="95" t="s">
         <v>585</v>
       </c>
-      <c r="F339" s="97"/>
-      <c r="G339" s="98"/>
+      <c r="F339" s="96"/>
+      <c r="G339" s="105"/>
       <c r="H339" s="5"/>
       <c r="O339" s="5"/>
       <c r="P339" s="5"/>
@@ -11798,16 +12187,16 @@
       <c r="A340" s="11" t="s">
         <v>168</v>
       </c>
-      <c r="B340" s="96" t="s">
+      <c r="B340" s="97" t="s">
         <v>586</v>
       </c>
-      <c r="C340" s="97"/>
-      <c r="D340" s="97"/>
-      <c r="E340" s="96" t="s">
+      <c r="C340" s="96"/>
+      <c r="D340" s="96"/>
+      <c r="E340" s="97" t="s">
         <v>587</v>
       </c>
-      <c r="F340" s="97"/>
-      <c r="G340" s="98"/>
+      <c r="F340" s="96"/>
+      <c r="G340" s="105"/>
       <c r="H340" s="5"/>
       <c r="O340" s="5"/>
       <c r="P340" s="5"/>
@@ -11826,16 +12215,16 @@
       <c r="A341" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B341" s="99" t="s">
+      <c r="B341" s="95" t="s">
         <v>586</v>
       </c>
-      <c r="C341" s="97"/>
-      <c r="D341" s="97"/>
-      <c r="E341" s="99" t="s">
+      <c r="C341" s="96"/>
+      <c r="D341" s="96"/>
+      <c r="E341" s="95" t="s">
         <v>391</v>
       </c>
-      <c r="F341" s="97"/>
-      <c r="G341" s="98"/>
+      <c r="F341" s="96"/>
+      <c r="G341" s="105"/>
       <c r="H341" s="5"/>
       <c r="O341" s="5"/>
       <c r="P341" s="5"/>
@@ -11854,16 +12243,16 @@
       <c r="A342" s="11" t="s">
         <v>175</v>
       </c>
-      <c r="B342" s="96" t="s">
+      <c r="B342" s="97" t="s">
         <v>588</v>
       </c>
-      <c r="C342" s="97"/>
-      <c r="D342" s="97"/>
-      <c r="E342" s="96" t="s">
+      <c r="C342" s="96"/>
+      <c r="D342" s="96"/>
+      <c r="E342" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="F342" s="97"/>
-      <c r="G342" s="98"/>
+      <c r="F342" s="96"/>
+      <c r="G342" s="105"/>
       <c r="H342" s="5"/>
       <c r="O342" s="5"/>
       <c r="P342" s="5"/>
@@ -11882,16 +12271,16 @@
       <c r="A343" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="B343" s="99" t="s">
+      <c r="B343" s="95" t="s">
         <v>588</v>
       </c>
-      <c r="C343" s="97"/>
-      <c r="D343" s="97"/>
-      <c r="E343" s="99" t="s">
+      <c r="C343" s="96"/>
+      <c r="D343" s="96"/>
+      <c r="E343" s="95" t="s">
         <v>589</v>
       </c>
-      <c r="F343" s="97"/>
-      <c r="G343" s="98"/>
+      <c r="F343" s="96"/>
+      <c r="G343" s="105"/>
       <c r="H343" s="5"/>
       <c r="N343" s="5"/>
       <c r="O343" s="5"/>
@@ -11911,16 +12300,16 @@
       <c r="A344" s="11" t="s">
         <v>182</v>
       </c>
-      <c r="B344" s="96" t="s">
+      <c r="B344" s="97" t="s">
         <v>590</v>
       </c>
-      <c r="C344" s="97"/>
-      <c r="D344" s="97"/>
-      <c r="E344" s="96" t="s">
+      <c r="C344" s="96"/>
+      <c r="D344" s="96"/>
+      <c r="E344" s="97" t="s">
         <v>392</v>
       </c>
-      <c r="F344" s="97"/>
-      <c r="G344" s="98"/>
+      <c r="F344" s="96"/>
+      <c r="G344" s="105"/>
       <c r="H344" s="5"/>
       <c r="N344" s="5"/>
       <c r="O344" s="5"/>
@@ -11940,16 +12329,16 @@
       <c r="A345" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="B345" s="99" t="s">
+      <c r="B345" s="95" t="s">
         <v>590</v>
       </c>
-      <c r="C345" s="97"/>
-      <c r="D345" s="97"/>
-      <c r="E345" s="99" t="s">
+      <c r="C345" s="96"/>
+      <c r="D345" s="96"/>
+      <c r="E345" s="95" t="s">
         <v>221</v>
       </c>
-      <c r="F345" s="97"/>
-      <c r="G345" s="98"/>
+      <c r="F345" s="96"/>
+      <c r="G345" s="105"/>
       <c r="H345" s="5"/>
       <c r="N345" s="5"/>
       <c r="O345" s="5"/>
@@ -11969,16 +12358,16 @@
       <c r="A346" s="11" t="s">
         <v>187</v>
       </c>
-      <c r="B346" s="96" t="s">
+      <c r="B346" s="97" t="s">
         <v>216</v>
       </c>
-      <c r="C346" s="97"/>
-      <c r="D346" s="97"/>
-      <c r="E346" s="96" t="s">
+      <c r="C346" s="96"/>
+      <c r="D346" s="96"/>
+      <c r="E346" s="97" t="s">
         <v>591</v>
       </c>
-      <c r="F346" s="97"/>
-      <c r="G346" s="98"/>
+      <c r="F346" s="96"/>
+      <c r="G346" s="105"/>
       <c r="H346" s="5"/>
       <c r="N346" s="5"/>
       <c r="O346" s="5"/>
@@ -11998,16 +12387,16 @@
       <c r="A347" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="B347" s="99" t="s">
+      <c r="B347" s="95" t="s">
         <v>216</v>
       </c>
-      <c r="C347" s="97"/>
-      <c r="D347" s="97"/>
-      <c r="E347" s="99" t="s">
+      <c r="C347" s="96"/>
+      <c r="D347" s="96"/>
+      <c r="E347" s="95" t="s">
         <v>189</v>
       </c>
-      <c r="F347" s="97"/>
-      <c r="G347" s="98"/>
+      <c r="F347" s="96"/>
+      <c r="G347" s="105"/>
       <c r="H347" s="5"/>
       <c r="N347" s="5"/>
       <c r="O347" s="5"/>
@@ -12027,16 +12416,16 @@
       <c r="A348" s="11" t="s">
         <v>193</v>
       </c>
-      <c r="B348" s="96" t="s">
+      <c r="B348" s="97" t="s">
         <v>592</v>
       </c>
-      <c r="C348" s="97"/>
-      <c r="D348" s="97"/>
-      <c r="E348" s="96" t="s">
+      <c r="C348" s="96"/>
+      <c r="D348" s="96"/>
+      <c r="E348" s="97" t="s">
         <v>593</v>
       </c>
-      <c r="F348" s="97"/>
-      <c r="G348" s="98"/>
+      <c r="F348" s="96"/>
+      <c r="G348" s="105"/>
       <c r="H348" s="5"/>
       <c r="N348" s="5"/>
       <c r="O348" s="5"/>
@@ -12056,16 +12445,16 @@
       <c r="A349" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="B349" s="99" t="s">
+      <c r="B349" s="95" t="s">
         <v>592</v>
       </c>
-      <c r="C349" s="97"/>
-      <c r="D349" s="97"/>
-      <c r="E349" s="99" t="s">
+      <c r="C349" s="96"/>
+      <c r="D349" s="96"/>
+      <c r="E349" s="95" t="s">
         <v>185</v>
       </c>
-      <c r="F349" s="97"/>
-      <c r="G349" s="98"/>
+      <c r="F349" s="96"/>
+      <c r="G349" s="105"/>
       <c r="H349" s="5"/>
       <c r="N349" s="5"/>
       <c r="O349" s="5"/>
@@ -12085,16 +12474,16 @@
       <c r="A350" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B350" s="96" t="s">
+      <c r="B350" s="97" t="s">
         <v>594</v>
       </c>
-      <c r="C350" s="97"/>
-      <c r="D350" s="97"/>
-      <c r="E350" s="96" t="s">
+      <c r="C350" s="96"/>
+      <c r="D350" s="96"/>
+      <c r="E350" s="97" t="s">
         <v>183</v>
       </c>
-      <c r="F350" s="97"/>
-      <c r="G350" s="98"/>
+      <c r="F350" s="96"/>
+      <c r="G350" s="105"/>
       <c r="H350" s="5"/>
       <c r="N350" s="5"/>
       <c r="O350" s="5"/>
@@ -12114,16 +12503,16 @@
       <c r="A351" s="65" t="s">
         <v>204</v>
       </c>
-      <c r="B351" s="102" t="s">
+      <c r="B351" s="100" t="s">
         <v>594</v>
       </c>
-      <c r="C351" s="103"/>
-      <c r="D351" s="103"/>
-      <c r="E351" s="102" t="s">
+      <c r="C351" s="101"/>
+      <c r="D351" s="101"/>
+      <c r="E351" s="100" t="s">
         <v>177</v>
       </c>
-      <c r="F351" s="103"/>
-      <c r="G351" s="105"/>
+      <c r="F351" s="101"/>
+      <c r="G351" s="117"/>
       <c r="H351" s="5"/>
       <c r="N351" s="5"/>
       <c r="O351" s="5"/>
@@ -31708,28 +32097,251 @@
     </row>
   </sheetData>
   <mergeCells count="291">
-    <mergeCell ref="E265:G265"/>
-    <mergeCell ref="E262:G262"/>
-    <mergeCell ref="E263:G263"/>
-    <mergeCell ref="B304:D304"/>
-    <mergeCell ref="B271:D271"/>
-    <mergeCell ref="B267:D267"/>
-    <mergeCell ref="B277:D277"/>
-    <mergeCell ref="B262:D262"/>
-    <mergeCell ref="B263:D263"/>
-    <mergeCell ref="B264:D264"/>
-    <mergeCell ref="B269:D269"/>
-    <mergeCell ref="B268:D268"/>
-    <mergeCell ref="B270:D270"/>
-    <mergeCell ref="D207:E207"/>
-    <mergeCell ref="D210:E210"/>
-    <mergeCell ref="D208:E208"/>
-    <mergeCell ref="B207:C207"/>
-    <mergeCell ref="B208:C208"/>
-    <mergeCell ref="B210:C210"/>
-    <mergeCell ref="B214:C214"/>
-    <mergeCell ref="E251:G251"/>
-    <mergeCell ref="E252:G252"/>
+    <mergeCell ref="H251:J251"/>
+    <mergeCell ref="H252:J252"/>
+    <mergeCell ref="H253:J253"/>
+    <mergeCell ref="H254:J254"/>
+    <mergeCell ref="H255:J255"/>
+    <mergeCell ref="H263:J263"/>
+    <mergeCell ref="E334:G334"/>
+    <mergeCell ref="E304:G304"/>
+    <mergeCell ref="E331:G331"/>
+    <mergeCell ref="E333:G333"/>
+    <mergeCell ref="E332:G332"/>
+    <mergeCell ref="H304:J304"/>
+    <mergeCell ref="E269:G269"/>
+    <mergeCell ref="E270:G270"/>
+    <mergeCell ref="E277:G277"/>
+    <mergeCell ref="E271:G271"/>
+    <mergeCell ref="H277:I277"/>
+    <mergeCell ref="E268:G268"/>
+    <mergeCell ref="E266:G266"/>
+    <mergeCell ref="E255:G255"/>
+    <mergeCell ref="H270:J270"/>
+    <mergeCell ref="H271:J271"/>
+    <mergeCell ref="H265:J265"/>
+    <mergeCell ref="H266:J266"/>
+    <mergeCell ref="H267:J267"/>
+    <mergeCell ref="H268:J268"/>
+    <mergeCell ref="H269:J269"/>
+    <mergeCell ref="H264:J264"/>
+    <mergeCell ref="H256:J256"/>
+    <mergeCell ref="H257:J257"/>
+    <mergeCell ref="H261:J261"/>
+    <mergeCell ref="H262:J262"/>
+    <mergeCell ref="H259:J259"/>
+    <mergeCell ref="H258:J258"/>
+    <mergeCell ref="H260:J260"/>
+    <mergeCell ref="B350:D350"/>
+    <mergeCell ref="B351:D351"/>
+    <mergeCell ref="E345:G345"/>
+    <mergeCell ref="E346:G346"/>
+    <mergeCell ref="A304:A305"/>
+    <mergeCell ref="A277:A278"/>
+    <mergeCell ref="E350:G350"/>
+    <mergeCell ref="E351:G351"/>
+    <mergeCell ref="E349:G349"/>
+    <mergeCell ref="E337:G337"/>
+    <mergeCell ref="E336:G336"/>
+    <mergeCell ref="E339:G339"/>
+    <mergeCell ref="E338:G338"/>
+    <mergeCell ref="E335:G335"/>
+    <mergeCell ref="B332:D332"/>
+    <mergeCell ref="B336:D336"/>
+    <mergeCell ref="E347:G347"/>
+    <mergeCell ref="E348:G348"/>
+    <mergeCell ref="B334:D334"/>
+    <mergeCell ref="B333:D333"/>
+    <mergeCell ref="B345:D345"/>
+    <mergeCell ref="B346:D346"/>
+    <mergeCell ref="B344:D344"/>
+    <mergeCell ref="H108:J108"/>
+    <mergeCell ref="H107:J107"/>
+    <mergeCell ref="E104:G104"/>
+    <mergeCell ref="E105:G105"/>
+    <mergeCell ref="H105:J105"/>
+    <mergeCell ref="H104:J104"/>
+    <mergeCell ref="H110:J110"/>
+    <mergeCell ref="H109:J109"/>
+    <mergeCell ref="H103:J103"/>
+    <mergeCell ref="H106:J106"/>
+    <mergeCell ref="E103:G103"/>
+    <mergeCell ref="E107:G107"/>
+    <mergeCell ref="E110:G110"/>
+    <mergeCell ref="E106:G106"/>
+    <mergeCell ref="E108:G108"/>
+    <mergeCell ref="E109:G109"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H97:J97"/>
+    <mergeCell ref="H98:J98"/>
+    <mergeCell ref="H95:J95"/>
+    <mergeCell ref="H92:J92"/>
+    <mergeCell ref="H93:J93"/>
+    <mergeCell ref="H94:J94"/>
+    <mergeCell ref="H91:J91"/>
+    <mergeCell ref="H90:J90"/>
+    <mergeCell ref="E92:G92"/>
+    <mergeCell ref="E91:G91"/>
+    <mergeCell ref="H79:J79"/>
+    <mergeCell ref="E79:G79"/>
+    <mergeCell ref="H80:J80"/>
+    <mergeCell ref="E80:G80"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="E67:G67"/>
+    <mergeCell ref="E66:G66"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="F1:F2"/>
+    <mergeCell ref="G1:G2"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="E63:G63"/>
+    <mergeCell ref="E64:G64"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="E101:G101"/>
+    <mergeCell ref="E93:G93"/>
+    <mergeCell ref="E94:G94"/>
+    <mergeCell ref="E95:G95"/>
+    <mergeCell ref="E96:G96"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B101:D101"/>
+    <mergeCell ref="B82:D82"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="B80:D80"/>
+    <mergeCell ref="E82:G82"/>
+    <mergeCell ref="E81:G81"/>
+    <mergeCell ref="E83:G83"/>
+    <mergeCell ref="E65:G65"/>
+    <mergeCell ref="E77:G77"/>
+    <mergeCell ref="E76:G76"/>
+    <mergeCell ref="E75:G75"/>
+    <mergeCell ref="E74:G74"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="H64:J64"/>
+    <mergeCell ref="H63:J63"/>
+    <mergeCell ref="H102:J102"/>
+    <mergeCell ref="H101:J101"/>
+    <mergeCell ref="H78:J78"/>
+    <mergeCell ref="H83:J83"/>
+    <mergeCell ref="H82:J82"/>
+    <mergeCell ref="H81:J81"/>
+    <mergeCell ref="H66:J66"/>
+    <mergeCell ref="H65:J65"/>
+    <mergeCell ref="H69:J69"/>
+    <mergeCell ref="H77:J77"/>
+    <mergeCell ref="H73:J73"/>
+    <mergeCell ref="H76:J76"/>
+    <mergeCell ref="H75:J75"/>
+    <mergeCell ref="H74:J74"/>
+    <mergeCell ref="E73:G73"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="H96:J96"/>
+    <mergeCell ref="H100:J100"/>
+    <mergeCell ref="H99:J99"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="H72:J72"/>
+    <mergeCell ref="H71:J71"/>
+    <mergeCell ref="H70:J70"/>
+    <mergeCell ref="E69:G69"/>
+    <mergeCell ref="E70:G70"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="H68:J68"/>
+    <mergeCell ref="E68:G68"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="H67:J67"/>
+    <mergeCell ref="E72:G72"/>
+    <mergeCell ref="E71:G71"/>
+    <mergeCell ref="B91:D91"/>
+    <mergeCell ref="B90:D90"/>
+    <mergeCell ref="A198:A199"/>
+    <mergeCell ref="D200:E200"/>
+    <mergeCell ref="D201:E201"/>
+    <mergeCell ref="D202:E202"/>
+    <mergeCell ref="B198:E198"/>
+    <mergeCell ref="F198:F199"/>
+    <mergeCell ref="B77:D77"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="B76:D76"/>
+    <mergeCell ref="B78:D78"/>
+    <mergeCell ref="B79:D79"/>
+    <mergeCell ref="E102:G102"/>
+    <mergeCell ref="E90:G90"/>
+    <mergeCell ref="E78:G78"/>
+    <mergeCell ref="B103:D103"/>
+    <mergeCell ref="B107:D107"/>
+    <mergeCell ref="B110:D110"/>
+    <mergeCell ref="B106:D106"/>
+    <mergeCell ref="B102:D102"/>
+    <mergeCell ref="B109:D109"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B96:D96"/>
+    <mergeCell ref="B95:D95"/>
+    <mergeCell ref="B105:D105"/>
+    <mergeCell ref="D199:E199"/>
+    <mergeCell ref="B199:C199"/>
+    <mergeCell ref="B200:C200"/>
+    <mergeCell ref="B201:C201"/>
+    <mergeCell ref="B202:C202"/>
+    <mergeCell ref="B203:C203"/>
+    <mergeCell ref="E264:G264"/>
+    <mergeCell ref="B217:C217"/>
+    <mergeCell ref="B215:C215"/>
+    <mergeCell ref="D217:E217"/>
+    <mergeCell ref="D218:E218"/>
+    <mergeCell ref="D215:E215"/>
+    <mergeCell ref="D219:E219"/>
+    <mergeCell ref="B219:C219"/>
+    <mergeCell ref="B261:D261"/>
+    <mergeCell ref="E261:G261"/>
+    <mergeCell ref="E259:G259"/>
+    <mergeCell ref="E253:G253"/>
+    <mergeCell ref="E254:G254"/>
+    <mergeCell ref="E256:G256"/>
+    <mergeCell ref="E257:G257"/>
+    <mergeCell ref="E258:G258"/>
+    <mergeCell ref="D203:E203"/>
+    <mergeCell ref="D204:E204"/>
+    <mergeCell ref="B341:D341"/>
+    <mergeCell ref="B342:D342"/>
+    <mergeCell ref="B343:D343"/>
+    <mergeCell ref="B337:D337"/>
+    <mergeCell ref="B339:D339"/>
+    <mergeCell ref="B338:D338"/>
+    <mergeCell ref="B340:D340"/>
+    <mergeCell ref="B335:D335"/>
+    <mergeCell ref="E343:G343"/>
+    <mergeCell ref="E340:G340"/>
+    <mergeCell ref="E341:G341"/>
+    <mergeCell ref="E342:G342"/>
+    <mergeCell ref="B256:D256"/>
+    <mergeCell ref="B204:C204"/>
+    <mergeCell ref="B218:C218"/>
+    <mergeCell ref="B251:D251"/>
+    <mergeCell ref="B216:C216"/>
+    <mergeCell ref="E344:G344"/>
+    <mergeCell ref="B104:D104"/>
+    <mergeCell ref="B92:D92"/>
+    <mergeCell ref="B93:D93"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="E97:G97"/>
+    <mergeCell ref="B97:D97"/>
+    <mergeCell ref="B98:D98"/>
+    <mergeCell ref="E98:G98"/>
+    <mergeCell ref="B100:D100"/>
+    <mergeCell ref="B99:D99"/>
+    <mergeCell ref="E100:G100"/>
+    <mergeCell ref="E99:G99"/>
+    <mergeCell ref="D209:E209"/>
+    <mergeCell ref="B209:C209"/>
+    <mergeCell ref="B206:C206"/>
+    <mergeCell ref="D206:E206"/>
+    <mergeCell ref="D205:E205"/>
+    <mergeCell ref="B205:C205"/>
     <mergeCell ref="B347:D347"/>
     <mergeCell ref="B349:D349"/>
     <mergeCell ref="B348:D348"/>
@@ -31754,251 +32366,28 @@
     <mergeCell ref="B266:D266"/>
     <mergeCell ref="B265:D265"/>
     <mergeCell ref="B331:D331"/>
-    <mergeCell ref="B256:D256"/>
-    <mergeCell ref="B204:C204"/>
-    <mergeCell ref="B218:C218"/>
-    <mergeCell ref="B251:D251"/>
-    <mergeCell ref="B216:C216"/>
-    <mergeCell ref="E344:G344"/>
-    <mergeCell ref="B104:D104"/>
-    <mergeCell ref="B92:D92"/>
-    <mergeCell ref="B93:D93"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="E97:G97"/>
-    <mergeCell ref="B97:D97"/>
-    <mergeCell ref="B98:D98"/>
-    <mergeCell ref="E98:G98"/>
-    <mergeCell ref="B100:D100"/>
-    <mergeCell ref="B99:D99"/>
-    <mergeCell ref="E100:G100"/>
-    <mergeCell ref="E99:G99"/>
-    <mergeCell ref="D209:E209"/>
-    <mergeCell ref="B209:C209"/>
-    <mergeCell ref="B206:C206"/>
-    <mergeCell ref="D206:E206"/>
-    <mergeCell ref="D205:E205"/>
-    <mergeCell ref="B205:C205"/>
-    <mergeCell ref="B341:D341"/>
-    <mergeCell ref="B342:D342"/>
-    <mergeCell ref="B343:D343"/>
-    <mergeCell ref="B337:D337"/>
-    <mergeCell ref="B339:D339"/>
-    <mergeCell ref="B338:D338"/>
-    <mergeCell ref="B340:D340"/>
-    <mergeCell ref="B335:D335"/>
-    <mergeCell ref="E343:G343"/>
-    <mergeCell ref="E340:G340"/>
-    <mergeCell ref="E341:G341"/>
-    <mergeCell ref="D199:E199"/>
-    <mergeCell ref="B199:C199"/>
-    <mergeCell ref="B200:C200"/>
-    <mergeCell ref="B201:C201"/>
-    <mergeCell ref="B202:C202"/>
-    <mergeCell ref="B203:C203"/>
-    <mergeCell ref="E264:G264"/>
-    <mergeCell ref="B217:C217"/>
-    <mergeCell ref="B215:C215"/>
-    <mergeCell ref="D217:E217"/>
-    <mergeCell ref="D218:E218"/>
-    <mergeCell ref="D215:E215"/>
-    <mergeCell ref="D219:E219"/>
-    <mergeCell ref="B219:C219"/>
-    <mergeCell ref="B261:D261"/>
-    <mergeCell ref="E261:G261"/>
-    <mergeCell ref="E259:G259"/>
-    <mergeCell ref="E253:G253"/>
-    <mergeCell ref="E254:G254"/>
-    <mergeCell ref="E256:G256"/>
-    <mergeCell ref="E257:G257"/>
-    <mergeCell ref="E258:G258"/>
-    <mergeCell ref="D203:E203"/>
-    <mergeCell ref="D204:E204"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="D200:E200"/>
-    <mergeCell ref="D201:E201"/>
-    <mergeCell ref="D202:E202"/>
-    <mergeCell ref="B198:E198"/>
-    <mergeCell ref="F198:F199"/>
-    <mergeCell ref="B77:D77"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B76:D76"/>
-    <mergeCell ref="B78:D78"/>
-    <mergeCell ref="B79:D79"/>
-    <mergeCell ref="E102:G102"/>
-    <mergeCell ref="E90:G90"/>
-    <mergeCell ref="E78:G78"/>
-    <mergeCell ref="B103:D103"/>
-    <mergeCell ref="B107:D107"/>
-    <mergeCell ref="B110:D110"/>
-    <mergeCell ref="B106:D106"/>
-    <mergeCell ref="B102:D102"/>
-    <mergeCell ref="B109:D109"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B96:D96"/>
-    <mergeCell ref="B95:D95"/>
-    <mergeCell ref="B105:D105"/>
-    <mergeCell ref="E73:G73"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="H96:J96"/>
-    <mergeCell ref="H100:J100"/>
-    <mergeCell ref="H99:J99"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="H72:J72"/>
-    <mergeCell ref="H71:J71"/>
-    <mergeCell ref="H70:J70"/>
-    <mergeCell ref="E69:G69"/>
-    <mergeCell ref="E70:G70"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="H68:J68"/>
-    <mergeCell ref="E68:G68"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="H67:J67"/>
-    <mergeCell ref="E72:G72"/>
-    <mergeCell ref="E71:G71"/>
-    <mergeCell ref="B91:D91"/>
-    <mergeCell ref="B90:D90"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="H64:J64"/>
-    <mergeCell ref="H63:J63"/>
-    <mergeCell ref="H102:J102"/>
-    <mergeCell ref="H101:J101"/>
-    <mergeCell ref="H78:J78"/>
-    <mergeCell ref="H83:J83"/>
-    <mergeCell ref="H82:J82"/>
-    <mergeCell ref="H81:J81"/>
-    <mergeCell ref="H66:J66"/>
-    <mergeCell ref="H65:J65"/>
-    <mergeCell ref="H69:J69"/>
-    <mergeCell ref="H77:J77"/>
-    <mergeCell ref="H73:J73"/>
-    <mergeCell ref="H76:J76"/>
-    <mergeCell ref="H75:J75"/>
-    <mergeCell ref="H74:J74"/>
-    <mergeCell ref="F1:F2"/>
-    <mergeCell ref="G1:G2"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="E63:G63"/>
-    <mergeCell ref="E64:G64"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="E101:G101"/>
-    <mergeCell ref="E93:G93"/>
-    <mergeCell ref="E94:G94"/>
-    <mergeCell ref="E95:G95"/>
-    <mergeCell ref="E96:G96"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B101:D101"/>
-    <mergeCell ref="B82:D82"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="B80:D80"/>
-    <mergeCell ref="E82:G82"/>
-    <mergeCell ref="E81:G81"/>
-    <mergeCell ref="E83:G83"/>
-    <mergeCell ref="E65:G65"/>
-    <mergeCell ref="E77:G77"/>
-    <mergeCell ref="E76:G76"/>
-    <mergeCell ref="E75:G75"/>
-    <mergeCell ref="E74:G74"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="H97:J97"/>
-    <mergeCell ref="H98:J98"/>
-    <mergeCell ref="H95:J95"/>
-    <mergeCell ref="H92:J92"/>
-    <mergeCell ref="H93:J93"/>
-    <mergeCell ref="H94:J94"/>
-    <mergeCell ref="H91:J91"/>
-    <mergeCell ref="H90:J90"/>
-    <mergeCell ref="E92:G92"/>
-    <mergeCell ref="E91:G91"/>
-    <mergeCell ref="H79:J79"/>
-    <mergeCell ref="E79:G79"/>
-    <mergeCell ref="H80:J80"/>
-    <mergeCell ref="E80:G80"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="E67:G67"/>
-    <mergeCell ref="E66:G66"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="H108:J108"/>
-    <mergeCell ref="H107:J107"/>
-    <mergeCell ref="E104:G104"/>
-    <mergeCell ref="E105:G105"/>
-    <mergeCell ref="H105:J105"/>
-    <mergeCell ref="H104:J104"/>
-    <mergeCell ref="H110:J110"/>
-    <mergeCell ref="H109:J109"/>
-    <mergeCell ref="H103:J103"/>
-    <mergeCell ref="H106:J106"/>
-    <mergeCell ref="E103:G103"/>
-    <mergeCell ref="E107:G107"/>
-    <mergeCell ref="E110:G110"/>
-    <mergeCell ref="E106:G106"/>
-    <mergeCell ref="E108:G108"/>
-    <mergeCell ref="E109:G109"/>
-    <mergeCell ref="E342:G342"/>
-    <mergeCell ref="B350:D350"/>
-    <mergeCell ref="B351:D351"/>
-    <mergeCell ref="E345:G345"/>
-    <mergeCell ref="E346:G346"/>
-    <mergeCell ref="A304:A305"/>
-    <mergeCell ref="A277:A278"/>
-    <mergeCell ref="E350:G350"/>
-    <mergeCell ref="E351:G351"/>
-    <mergeCell ref="E349:G349"/>
-    <mergeCell ref="E337:G337"/>
-    <mergeCell ref="E336:G336"/>
-    <mergeCell ref="E339:G339"/>
-    <mergeCell ref="E338:G338"/>
-    <mergeCell ref="E335:G335"/>
-    <mergeCell ref="B332:D332"/>
-    <mergeCell ref="B336:D336"/>
-    <mergeCell ref="E347:G347"/>
-    <mergeCell ref="E348:G348"/>
-    <mergeCell ref="B334:D334"/>
-    <mergeCell ref="B333:D333"/>
-    <mergeCell ref="B345:D345"/>
-    <mergeCell ref="B346:D346"/>
-    <mergeCell ref="B344:D344"/>
-    <mergeCell ref="H267:J267"/>
-    <mergeCell ref="H268:J268"/>
-    <mergeCell ref="H269:J269"/>
-    <mergeCell ref="H264:J264"/>
-    <mergeCell ref="H256:J256"/>
-    <mergeCell ref="H257:J257"/>
-    <mergeCell ref="H261:J261"/>
-    <mergeCell ref="H262:J262"/>
-    <mergeCell ref="H259:J259"/>
-    <mergeCell ref="H258:J258"/>
-    <mergeCell ref="H260:J260"/>
-    <mergeCell ref="H251:J251"/>
-    <mergeCell ref="H252:J252"/>
-    <mergeCell ref="H253:J253"/>
-    <mergeCell ref="H254:J254"/>
-    <mergeCell ref="H255:J255"/>
-    <mergeCell ref="H263:J263"/>
-    <mergeCell ref="E334:G334"/>
-    <mergeCell ref="E304:G304"/>
-    <mergeCell ref="E331:G331"/>
-    <mergeCell ref="E333:G333"/>
-    <mergeCell ref="E332:G332"/>
-    <mergeCell ref="H304:J304"/>
-    <mergeCell ref="E269:G269"/>
-    <mergeCell ref="E270:G270"/>
-    <mergeCell ref="E277:G277"/>
-    <mergeCell ref="E271:G271"/>
-    <mergeCell ref="H277:I277"/>
-    <mergeCell ref="E268:G268"/>
-    <mergeCell ref="E266:G266"/>
-    <mergeCell ref="E255:G255"/>
-    <mergeCell ref="H270:J270"/>
-    <mergeCell ref="H271:J271"/>
-    <mergeCell ref="H265:J265"/>
-    <mergeCell ref="H266:J266"/>
+    <mergeCell ref="D207:E207"/>
+    <mergeCell ref="D210:E210"/>
+    <mergeCell ref="D208:E208"/>
+    <mergeCell ref="B207:C207"/>
+    <mergeCell ref="B208:C208"/>
+    <mergeCell ref="B210:C210"/>
+    <mergeCell ref="B214:C214"/>
+    <mergeCell ref="E251:G251"/>
+    <mergeCell ref="E252:G252"/>
+    <mergeCell ref="E265:G265"/>
+    <mergeCell ref="E262:G262"/>
+    <mergeCell ref="E263:G263"/>
+    <mergeCell ref="B304:D304"/>
+    <mergeCell ref="B271:D271"/>
+    <mergeCell ref="B267:D267"/>
+    <mergeCell ref="B277:D277"/>
+    <mergeCell ref="B262:D262"/>
+    <mergeCell ref="B263:D263"/>
+    <mergeCell ref="B264:D264"/>
+    <mergeCell ref="B269:D269"/>
+    <mergeCell ref="B268:D268"/>
+    <mergeCell ref="B270:D270"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -33350,8 +33739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -33989,4 +34378,755 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="59" t="s">
+        <v>630</v>
+      </c>
+      <c r="B1" s="42" t="s">
+        <v>631</v>
+      </c>
+      <c r="C1" s="42" t="s">
+        <v>632</v>
+      </c>
+      <c r="D1" s="42" t="s">
+        <v>633</v>
+      </c>
+      <c r="E1" s="42" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>629</v>
+      </c>
+      <c r="B2" s="120" t="s">
+        <v>636</v>
+      </c>
+      <c r="C2" s="121" t="s">
+        <v>635</v>
+      </c>
+      <c r="D2" s="121"/>
+      <c r="E2" s="121"/>
+      <c r="H2" s="10"/>
+      <c r="I2" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>637</v>
+      </c>
+      <c r="C3" s="121" t="s">
+        <v>638</v>
+      </c>
+      <c r="D3" s="121"/>
+      <c r="E3" s="121"/>
+      <c r="H3" s="10"/>
+      <c r="I3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B4" s="120" t="s">
+        <v>639</v>
+      </c>
+      <c r="C4" s="121" t="s">
+        <v>640</v>
+      </c>
+      <c r="D4" s="121" t="s">
+        <v>641</v>
+      </c>
+      <c r="E4" s="121" t="s">
+        <v>642</v>
+      </c>
+      <c r="H4" s="94"/>
+      <c r="I4" s="94"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B5" s="121" t="s">
+        <v>643</v>
+      </c>
+      <c r="C5" s="121" t="s">
+        <v>644</v>
+      </c>
+      <c r="D5" s="121" t="s">
+        <v>645</v>
+      </c>
+      <c r="E5" s="121"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B6" s="121" t="s">
+        <v>646</v>
+      </c>
+      <c r="C6" s="121" t="s">
+        <v>647</v>
+      </c>
+      <c r="D6" s="121" t="s">
+        <v>648</v>
+      </c>
+      <c r="E6" s="121"/>
+      <c r="H6" s="94"/>
+      <c r="I6" s="94"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B7" s="121" t="s">
+        <v>649</v>
+      </c>
+      <c r="C7" s="121" t="s">
+        <v>650</v>
+      </c>
+      <c r="D7" s="121" t="s">
+        <v>651</v>
+      </c>
+      <c r="E7" s="121"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B8" s="121" t="s">
+        <v>652</v>
+      </c>
+      <c r="C8" s="121" t="s">
+        <v>653</v>
+      </c>
+      <c r="D8" s="121" t="s">
+        <v>654</v>
+      </c>
+      <c r="E8" s="121"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B9" s="121" t="s">
+        <v>655</v>
+      </c>
+      <c r="C9" s="121" t="s">
+        <v>656</v>
+      </c>
+      <c r="D9" s="121" t="s">
+        <v>657</v>
+      </c>
+      <c r="E9" s="121"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B10" s="120" t="s">
+        <v>658</v>
+      </c>
+      <c r="C10" s="121" t="s">
+        <v>659</v>
+      </c>
+      <c r="D10" s="121" t="s">
+        <v>660</v>
+      </c>
+      <c r="E10" s="121"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B11" s="120" t="s">
+        <v>661</v>
+      </c>
+      <c r="C11" s="121" t="s">
+        <v>662</v>
+      </c>
+      <c r="D11" s="121" t="s">
+        <v>663</v>
+      </c>
+      <c r="E11" s="121"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B12" s="120" t="s">
+        <v>664</v>
+      </c>
+      <c r="C12" s="121" t="s">
+        <v>665</v>
+      </c>
+      <c r="D12" s="121"/>
+      <c r="E12" s="121"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B13" s="120" t="s">
+        <v>666</v>
+      </c>
+      <c r="C13" s="121" t="s">
+        <v>667</v>
+      </c>
+      <c r="D13" s="121" t="s">
+        <v>668</v>
+      </c>
+      <c r="E13" s="121"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B14" s="120" t="s">
+        <v>669</v>
+      </c>
+      <c r="C14" s="121" t="s">
+        <v>670</v>
+      </c>
+      <c r="D14" s="121" t="s">
+        <v>671</v>
+      </c>
+      <c r="E14" s="121"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B15" s="120" t="s">
+        <v>672</v>
+      </c>
+      <c r="C15" s="121" t="s">
+        <v>673</v>
+      </c>
+      <c r="D15" s="121" t="s">
+        <v>674</v>
+      </c>
+      <c r="E15" s="121"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B16" s="120" t="s">
+        <v>675</v>
+      </c>
+      <c r="C16" s="121" t="s">
+        <v>676</v>
+      </c>
+      <c r="D16" s="121"/>
+      <c r="E16" s="121"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="94" t="s">
+        <v>629</v>
+      </c>
+      <c r="B17" s="120" t="s">
+        <v>677</v>
+      </c>
+      <c r="C17" s="121" t="s">
+        <v>678</v>
+      </c>
+      <c r="D17" s="121" t="s">
+        <v>679</v>
+      </c>
+      <c r="E17" s="121"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="5"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>755</v>
+      </c>
+      <c r="B18" s="120" t="s">
+        <v>680</v>
+      </c>
+      <c r="C18" s="121" t="s">
+        <v>681</v>
+      </c>
+      <c r="D18" s="121" t="s">
+        <v>682</v>
+      </c>
+      <c r="E18" s="121"/>
+      <c r="H18" s="10"/>
+      <c r="I18" s="94"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B19" s="120" t="s">
+        <v>683</v>
+      </c>
+      <c r="C19" s="121" t="s">
+        <v>684</v>
+      </c>
+      <c r="D19" s="121" t="s">
+        <v>685</v>
+      </c>
+      <c r="E19" s="121"/>
+      <c r="H19" s="10"/>
+      <c r="I19" s="94"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B20" s="120" t="s">
+        <v>686</v>
+      </c>
+      <c r="C20" s="121" t="s">
+        <v>687</v>
+      </c>
+      <c r="D20" s="121" t="s">
+        <v>688</v>
+      </c>
+      <c r="E20" s="121"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="94"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B21" s="120" t="s">
+        <v>689</v>
+      </c>
+      <c r="C21" s="121" t="s">
+        <v>690</v>
+      </c>
+      <c r="D21" s="121" t="s">
+        <v>691</v>
+      </c>
+      <c r="E21" s="121"/>
+      <c r="H21" s="10"/>
+      <c r="I21" s="94"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B22" s="120" t="s">
+        <v>692</v>
+      </c>
+      <c r="C22" s="121" t="s">
+        <v>693</v>
+      </c>
+      <c r="D22" s="121" t="s">
+        <v>694</v>
+      </c>
+      <c r="E22" s="121" t="s">
+        <v>695</v>
+      </c>
+      <c r="H22" s="10"/>
+      <c r="I22" s="94"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B23" s="120" t="s">
+        <v>696</v>
+      </c>
+      <c r="C23" s="121" t="s">
+        <v>697</v>
+      </c>
+      <c r="D23" s="121" t="s">
+        <v>698</v>
+      </c>
+      <c r="E23" s="121"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="94"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B24" s="121" t="s">
+        <v>699</v>
+      </c>
+      <c r="C24" s="121" t="s">
+        <v>700</v>
+      </c>
+      <c r="D24" s="121" t="s">
+        <v>701</v>
+      </c>
+      <c r="E24" s="121"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="94"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B25" s="121" t="s">
+        <v>702</v>
+      </c>
+      <c r="C25" s="121" t="s">
+        <v>703</v>
+      </c>
+      <c r="D25" s="121" t="s">
+        <v>704</v>
+      </c>
+      <c r="E25" s="121"/>
+      <c r="H25" s="94"/>
+      <c r="I25" s="94"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B26" s="121" t="s">
+        <v>705</v>
+      </c>
+      <c r="C26" s="121" t="s">
+        <v>706</v>
+      </c>
+      <c r="D26" s="121"/>
+      <c r="E26" s="121"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="94"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B27" s="121" t="s">
+        <v>707</v>
+      </c>
+      <c r="C27" s="121" t="s">
+        <v>708</v>
+      </c>
+      <c r="D27" s="121"/>
+      <c r="E27" s="121"/>
+      <c r="H27" s="94"/>
+      <c r="I27" s="94"/>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A28" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B28" s="121" t="s">
+        <v>709</v>
+      </c>
+      <c r="C28" s="121" t="s">
+        <v>710</v>
+      </c>
+      <c r="D28" s="121" t="s">
+        <v>711</v>
+      </c>
+      <c r="E28" s="121"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B29" s="121" t="s">
+        <v>712</v>
+      </c>
+      <c r="C29" s="121" t="s">
+        <v>713</v>
+      </c>
+      <c r="D29" s="121" t="s">
+        <v>714</v>
+      </c>
+      <c r="E29" s="121" t="s">
+        <v>715</v>
+      </c>
+      <c r="H29" s="10"/>
+      <c r="I29" s="94"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A30" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B30" s="120" t="s">
+        <v>716</v>
+      </c>
+      <c r="C30" s="121" t="s">
+        <v>717</v>
+      </c>
+      <c r="D30" s="121"/>
+      <c r="E30" s="121"/>
+      <c r="H30" s="94"/>
+      <c r="I30" s="94"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" s="94" t="s">
+        <v>755</v>
+      </c>
+      <c r="B31" s="121" t="s">
+        <v>718</v>
+      </c>
+      <c r="C31" s="121" t="s">
+        <v>719</v>
+      </c>
+      <c r="D31" s="121"/>
+      <c r="E31" s="121"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>96</v>
+      </c>
+      <c r="B32" s="120" t="s">
+        <v>720</v>
+      </c>
+      <c r="C32" s="121" t="s">
+        <v>721</v>
+      </c>
+      <c r="D32" s="121" t="s">
+        <v>722</v>
+      </c>
+      <c r="E32" s="121"/>
+      <c r="H32" s="94"/>
+      <c r="I32" s="5"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B33" s="120" t="s">
+        <v>723</v>
+      </c>
+      <c r="C33" s="121" t="s">
+        <v>724</v>
+      </c>
+      <c r="D33" s="121"/>
+      <c r="E33" s="121"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="5"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A34" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B34" s="121" t="s">
+        <v>725</v>
+      </c>
+      <c r="C34" s="121" t="s">
+        <v>726</v>
+      </c>
+      <c r="D34" s="121"/>
+      <c r="E34" s="121"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="5"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B35" s="121" t="s">
+        <v>727</v>
+      </c>
+      <c r="C35" s="121" t="s">
+        <v>728</v>
+      </c>
+      <c r="D35" s="121" t="s">
+        <v>729</v>
+      </c>
+      <c r="E35" s="121"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="121" t="s">
+        <v>730</v>
+      </c>
+      <c r="C36" s="121" t="s">
+        <v>731</v>
+      </c>
+      <c r="D36" s="121"/>
+      <c r="E36" s="121"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="5"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A37" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="121" t="s">
+        <v>732</v>
+      </c>
+      <c r="C37" s="121" t="s">
+        <v>733</v>
+      </c>
+      <c r="D37" s="121"/>
+      <c r="E37" s="121"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="5"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A38" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B38" s="121" t="s">
+        <v>734</v>
+      </c>
+      <c r="C38" s="121" t="s">
+        <v>735</v>
+      </c>
+      <c r="D38" s="121"/>
+      <c r="E38" s="121"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B39" s="120" t="s">
+        <v>736</v>
+      </c>
+      <c r="C39" s="121" t="s">
+        <v>737</v>
+      </c>
+      <c r="D39" s="121" t="s">
+        <v>738</v>
+      </c>
+      <c r="E39" s="121"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="94" t="s">
+        <v>96</v>
+      </c>
+      <c r="B40" s="120" t="s">
+        <v>739</v>
+      </c>
+      <c r="C40" s="121" t="s">
+        <v>740</v>
+      </c>
+      <c r="D40" s="121"/>
+      <c r="E40" s="121"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>756</v>
+      </c>
+      <c r="B41" s="121" t="s">
+        <v>741</v>
+      </c>
+      <c r="C41" s="121" t="s">
+        <v>742</v>
+      </c>
+      <c r="D41" s="121" t="s">
+        <v>743</v>
+      </c>
+      <c r="E41" s="121"/>
+      <c r="H41" s="93"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A42" s="94" t="s">
+        <v>756</v>
+      </c>
+      <c r="B42" s="121" t="s">
+        <v>744</v>
+      </c>
+      <c r="C42" s="121" t="s">
+        <v>745</v>
+      </c>
+      <c r="D42" s="121" t="s">
+        <v>746</v>
+      </c>
+      <c r="E42" s="121" t="s">
+        <v>747</v>
+      </c>
+      <c r="H42" s="94"/>
+      <c r="I42" s="94"/>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A43" s="94" t="s">
+        <v>756</v>
+      </c>
+      <c r="B43" s="121" t="s">
+        <v>748</v>
+      </c>
+      <c r="C43" s="121" t="s">
+        <v>749</v>
+      </c>
+      <c r="D43" s="121" t="s">
+        <v>750</v>
+      </c>
+      <c r="E43" s="121"/>
+      <c r="H43" s="93"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A44" s="94" t="s">
+        <v>756</v>
+      </c>
+      <c r="B44" s="121" t="s">
+        <v>751</v>
+      </c>
+      <c r="C44" s="121" t="s">
+        <v>752</v>
+      </c>
+      <c r="D44" s="121" t="s">
+        <v>753</v>
+      </c>
+      <c r="E44" s="121" t="s">
+        <v>754</v>
+      </c>
+      <c r="H44" s="93"/>
+      <c r="I44" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>